<commit_message>
efficiencies using hourly regression with FE
</commit_message>
<xml_diff>
--- a/hourly datasets/PlantID_year-4final.xlsx
+++ b/hourly datasets/PlantID_year-4final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,3373 +472,3410 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6025</v>
+        <v>1384</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2448161647470965</v>
+        <v>0.3665293828999165</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001002218899688696</v>
+        <v>0.0006107359454498041</v>
       </c>
       <c r="D2" t="n">
-        <v>-90.62883501915448</v>
+        <v>98.65640692366263</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.09279425972977341</v>
+        <v>0.05905599163781375</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.08886560289615723</v>
+        <v>0.06145003627659365</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6041</v>
+        <v>1552</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3757212708017496</v>
+        <v>0.3160941919946067</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0009167539911669381</v>
+        <v>0.0006117811466514816</v>
       </c>
       <c r="D3" t="n">
-        <v>43.71420809488485</v>
+        <v>16.04793332653465</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>6.03821814669243e-58</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03827835578663632</v>
+        <v>0.008618752172605049</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04187199369673921</v>
+        <v>0.01101689393118274</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6052</v>
+        <v>1570</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3936250586438326</v>
+        <v>0.3130192018845155</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0008189211234084841</v>
+        <v>0.0007591052905219355</v>
       </c>
       <c r="D4" t="n">
-        <v>70.79920266612842</v>
+        <v>8.882605649035233</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>6.544624082440386e-19</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05637389403603604</v>
+        <v>0.005255011597256592</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05958403113150562</v>
+        <v>0.008230654286348759</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6061</v>
+        <v>1571</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3068127554957153</v>
+        <v>0.4005593312717744</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0007899999066474135</v>
+        <v>0.0006316029741617812</v>
       </c>
       <c r="D5" t="n">
-        <v>-36.49790376141799</v>
+        <v>149.2756782125468</v>
       </c>
       <c r="E5" t="n">
-        <v>2.119991257636926e-290</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.03038172412245468</v>
+        <v>0.09304504132130444</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.02728495700623831</v>
+        <v>0.0955208833368187</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6073</v>
+        <v>1573</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3519881527218555</v>
+        <v>0.3658962532800888</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0009034921745070998</v>
+        <v>0.0006141135063816767</v>
       </c>
       <c r="D6" t="n">
-        <v>18.08765711856789</v>
+        <v>97.08284171871267</v>
       </c>
       <c r="E6" t="n">
-        <v>4.748841224614624e-73</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01457123059445524</v>
+        <v>0.05841624210990516</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0181128827291322</v>
+        <v>0.06082352656484677</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6090</v>
+        <v>1606</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3260000557756663</v>
+        <v>0.3374977954227021</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0008378138028760602</v>
+        <v>0.0008024752362747829</v>
       </c>
       <c r="D7" t="n">
-        <v>-11.51334610540241</v>
+        <v>38.90640491901541</v>
       </c>
       <c r="E7" t="n">
-        <v>1.163313445459372e-30</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.01128813809505808</v>
+        <v>0.02964860147151334</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.008003942473732864</v>
+        <v>0.03279425148846519</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6094</v>
+        <v>1619</v>
       </c>
       <c r="B8" t="n">
-        <v>0.395919770412069</v>
+        <v>0.4126961685385792</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0008500748079846366</v>
+        <v>0.0006628514750943055</v>
       </c>
       <c r="D8" t="n">
-        <v>70.90396490504695</v>
+        <v>160.5484842297828</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.05860754522367448</v>
+        <v>0.1051206325564283</v>
       </c>
       <c r="G8" t="n">
-        <v>0.06193980348033992</v>
+        <v>0.1077189666353045</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6101</v>
+        <v>1702</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2765775200924052</v>
+        <v>0.4146733048530299</v>
       </c>
       <c r="C9" t="n">
-        <v>0.001059020237000586</v>
+        <v>0.0006268114604997905</v>
       </c>
       <c r="D9" t="n">
-        <v>-55.77662626632503</v>
+        <v>172.9338768373609</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.06114423383657255</v>
+        <v>0.1071684061113791</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.05699291809874072</v>
+        <v>0.1096254657092551</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6113</v>
+        <v>1710</v>
       </c>
       <c r="B10" t="n">
-        <v>0.4030887202535611</v>
+        <v>0.3737150348923871</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0008127816468397578</v>
+        <v>0.0006126343477937738</v>
       </c>
       <c r="D10" t="n">
-        <v>82.97754317623739</v>
+        <v>110.0797991371773</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0658495888934832</v>
+        <v>0.06623792282427339</v>
       </c>
       <c r="G10" t="n">
-        <v>0.06903565949351546</v>
+        <v>0.06863940907507514</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>6124</v>
+        <v>1720</v>
       </c>
       <c r="B11" t="n">
-        <v>0.4785952825243284</v>
+        <v>0.3633239760919307</v>
       </c>
       <c r="C11" t="n">
-        <v>0.001116751518507034</v>
+        <v>0.0006220325955734766</v>
       </c>
       <c r="D11" t="n">
-        <v>128.0044701934885</v>
+        <v>91.71160411075147</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1407603764717607</v>
+        <v>0.05582844376799403</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1451379964567726</v>
+        <v>0.05826677053044169</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6155</v>
+        <v>1723</v>
       </c>
       <c r="B12" t="n">
-        <v>0.3383700233956937</v>
+        <v>0.3662065579319304</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0007990824661658496</v>
+        <v>0.0006188806144854979</v>
       </c>
       <c r="D12" t="n">
-        <v>3.408818802772378</v>
+        <v>96.8364294930131</v>
       </c>
       <c r="E12" t="n">
-        <v>0.000652615362529179</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.001157742147794933</v>
+        <v>0.05871720338701706</v>
       </c>
       <c r="G12" t="n">
-        <v>0.004290112523468808</v>
+        <v>0.06114317459141801</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6195</v>
+        <v>1912</v>
       </c>
       <c r="B13" t="n">
-        <v>0.3730738631312597</v>
+        <v>0.2788859615921641</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0008639059352113297</v>
+        <v>0.000618134924452719</v>
       </c>
       <c r="D13" t="n">
-        <v>43.32389157859219</v>
+        <v>-44.31137324072009</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.03573452921815815</v>
+        <v>-0.02860193142486761</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03912100492423772</v>
+        <v>-0.02617888327622989</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6639</v>
+        <v>2049</v>
       </c>
       <c r="B14" t="n">
-        <v>0.3332312664407623</v>
+        <v>0.3649922995625561</v>
       </c>
       <c r="C14" t="n">
-        <v>0.000832542114778049</v>
+        <v>0.0006141597508830938</v>
       </c>
       <c r="D14" t="n">
-        <v>-2.900549505466504</v>
+        <v>95.60367727682612</v>
       </c>
       <c r="E14" t="n">
-        <v>0.003725617796395186</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.00404659502978618</v>
+        <v>0.05751219775467416</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0007830642088128357</v>
+        <v>0.05991966348501231</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6705</v>
+        <v>2076</v>
       </c>
       <c r="B15" t="n">
-        <v>0.3042545153497039</v>
+        <v>0.3549782372858382</v>
       </c>
       <c r="C15" t="n">
-        <v>0.001008813915237866</v>
+        <v>0.000662509235246253</v>
       </c>
       <c r="D15" t="n">
-        <v>-31.11731533060397</v>
+        <v>73.51122935670935</v>
       </c>
       <c r="E15" t="n">
-        <v>6.433878567689015e-212</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.03336883522191087</v>
+        <v>0.04740337208250715</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.02941432619880485</v>
+        <v>0.05000036460374368</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>8002</v>
+        <v>2079</v>
       </c>
       <c r="B16" t="n">
-        <v>0.2777718032635754</v>
+        <v>0.3507008135742782</v>
       </c>
       <c r="C16" t="n">
-        <v>0.001262276238159464</v>
+        <v>0.0006315944660520727</v>
       </c>
       <c r="D16" t="n">
-        <v>-45.84915016769496</v>
+        <v>70.33697573262587</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.06034832824447925</v>
+        <v>0.04318654029942284</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.05540025734849349</v>
+        <v>0.04566234896370802</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>8006</v>
+        <v>2080</v>
       </c>
       <c r="B17" t="n">
-        <v>0.3309064223609268</v>
+        <v>0.2997902999195626</v>
       </c>
       <c r="C17" t="n">
-        <v>0.001098310544721957</v>
+        <v>0.000613176145701226</v>
       </c>
       <c r="D17" t="n">
-        <v>-4.315422192668558</v>
+        <v>-10.57782346658769</v>
       </c>
       <c r="E17" t="n">
-        <v>1.593975093192906e-05</v>
+        <v>3.791777768500555e-26</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.006892339762554356</v>
+        <v>-0.00768787405458864</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.002587007635715699</v>
+        <v>-0.005284263991711806</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8066</v>
+        <v>2094</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2977368539158541</v>
+        <v>0.3390584362905549</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0008655459316827758</v>
+        <v>0.0006124136183540415</v>
       </c>
       <c r="D18" t="n">
-        <v>-43.79807097065938</v>
+        <v>53.52929191213788</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.0396056943565789</v>
+        <v>0.03158175684486646</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.03621278993183652</v>
+        <v>0.03398237785081771</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8102</v>
+        <v>2103</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3418029187854177</v>
+        <v>0.3387128825948262</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0008588780887069929</v>
+        <v>0.0006102339400881733</v>
       </c>
       <c r="D19" t="n">
-        <v>7.168447776592772</v>
+        <v>53.15422745484555</v>
       </c>
       <c r="E19" t="n">
-        <v>7.619190220306497e-13</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.004473439347986925</v>
+        <v>0.03124047524668295</v>
       </c>
       <c r="G19" t="n">
-        <v>0.00784020610272486</v>
+        <v>0.03363255205754376</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>8226</v>
+        <v>2104</v>
       </c>
       <c r="B20" t="n">
-        <v>0.3493137357777542</v>
+        <v>0.3328729616331672</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0008640472313835661</v>
+        <v>0.0006655871724962362</v>
       </c>
       <c r="D20" t="n">
-        <v>15.81816273608896</v>
+        <v>39.95959325764318</v>
       </c>
       <c r="E20" t="n">
-        <v>2.583787158706008e-56</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.01197412492706299</v>
+        <v>0.02529206377429429</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01536115450832173</v>
+        <v>0.02790112160661449</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6018</v>
+        <v>2107</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3356460960600618</v>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+        <v>0.336842071899995</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0006276429177020309</v>
+      </c>
+      <c r="D21" t="n">
+        <v>48.69919200106881</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.02933554352963788</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.03179586238492658</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3403</v>
+        <v>2161</v>
       </c>
       <c r="B22" t="n">
-        <v>0.370765901699259</v>
+        <v>0.337979025612808</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0006475857901697739</v>
+        <v>0.0006217423096309143</v>
       </c>
       <c r="D22" t="n">
-        <v>136.5199105479613</v>
+        <v>50.99002621988988</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.08713909952108172</v>
+        <v>0.03048406223974916</v>
       </c>
       <c r="G22" t="n">
-        <v>0.08967760877113508</v>
+        <v>0.03292125110044127</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3406</v>
+        <v>2167</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3501866673731518</v>
+        <v>0.3328386809912138</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0006593091279379863</v>
+        <v>0.0006096169843225522</v>
       </c>
       <c r="D23" t="n">
-        <v>102.8790850084834</v>
+        <v>43.57213255470374</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.06653688769777037</v>
+        <v>0.02536748285603247</v>
       </c>
       <c r="G23" t="n">
-        <v>0.06912135194223197</v>
+        <v>0.02775714124096952</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3942</v>
+        <v>2168</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3170316250839023</v>
+        <v>0.3372448890413768</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0006666442870487429</v>
+        <v>0.0006112053084135866</v>
       </c>
       <c r="D24" t="n">
-        <v>52.01286233810682</v>
+        <v>50.66795015089831</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.03336746864984583</v>
+        <v>0.02977057784333822</v>
       </c>
       <c r="G24" t="n">
-        <v>0.03598068641165744</v>
+        <v>0.03216646235398985</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3943</v>
+        <v>2364</v>
       </c>
       <c r="B25" t="n">
-        <v>0.343413833987481</v>
+        <v>0.3581179893123497</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0006438067990815468</v>
+        <v>0.0006134535844232558</v>
       </c>
       <c r="D25" t="n">
-        <v>94.83634922997577</v>
+        <v>84.507812303968</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.05979443855291899</v>
+        <v>0.05063927156744941</v>
       </c>
       <c r="G25" t="n">
-        <v>0.06231813431574185</v>
+        <v>0.05304396917182436</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3944</v>
+        <v>2378</v>
       </c>
       <c r="B26" t="n">
-        <v>0.3326618978584649</v>
+        <v>0.3349294202078384</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0006751880272081403</v>
+        <v>0.0006222434685155239</v>
       </c>
       <c r="D26" t="n">
-        <v>74.50420961005429</v>
+        <v>46.04797432985956</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.04898099587211729</v>
+        <v>0.02743347457988707</v>
       </c>
       <c r="G26" t="n">
-        <v>0.05162770473851136</v>
+        <v>0.02987262795036416</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3945</v>
+        <v>2516</v>
       </c>
       <c r="B27" t="n">
-        <v>0.2860037937887199</v>
+        <v>0.351128210801633</v>
       </c>
       <c r="C27" t="n">
-        <v>0.001008425664765448</v>
+        <v>0.0006156238713242021</v>
       </c>
       <c r="D27" t="n">
-        <v>3.61578087802569</v>
+        <v>72.85591730295354</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0002995374199278849</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.001669752991850004</v>
+        <v>0.04364523936595313</v>
       </c>
       <c r="G27" t="n">
-        <v>0.005622739479288498</v>
+        <v>0.04605844435188722</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>3946</v>
+        <v>2517</v>
       </c>
       <c r="B28" t="n">
-        <v>0.309067169312479</v>
+        <v>0.3619971564567163</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0007771150920475083</v>
+        <v>0.0006256185907056824</v>
       </c>
       <c r="D28" t="n">
-        <v>34.3702265374297</v>
+        <v>89.06510826532786</v>
       </c>
       <c r="E28" t="n">
-        <v>6.455322367069114e-258</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.02518649240761617</v>
+        <v>0.05449459570053741</v>
       </c>
       <c r="G28" t="n">
-        <v>0.02823275111104061</v>
+        <v>0.05694697932746948</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3947</v>
+        <v>2527</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3846957405179192</v>
+        <v>0.3510652415294904</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0006830843747546941</v>
+        <v>0.0006586054792445435</v>
       </c>
       <c r="D29" t="n">
-        <v>149.8177922771542</v>
+        <v>68.00561792797852</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1009993618552818</v>
+        <v>0.04349802755923039</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1036770240742553</v>
+        <v>0.04607971761432484</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3948</v>
+        <v>2535</v>
       </c>
       <c r="B30" t="n">
-        <v>0.3644119098687807</v>
+        <v>0.3181865703299488</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0006182866883436681</v>
+        <v>0.0006087605012391305</v>
       </c>
       <c r="D30" t="n">
-        <v>132.7124841316672</v>
+        <v>19.56467504542886</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>3.243577746225265e-85</v>
       </c>
       <c r="F30" t="n">
-        <v>0.08084253331832168</v>
+        <v>0.0107170508733759</v>
       </c>
       <c r="G30" t="n">
-        <v>0.08326619131293857</v>
+        <v>0.01310335190109606</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3954</v>
+        <v>2554</v>
       </c>
       <c r="B31" t="n">
-        <v>0.3513286346488912</v>
+        <v>0.3993410994228161</v>
       </c>
       <c r="C31" t="n">
-        <v>0.000644610337014806</v>
+        <v>0.0006175511633282125</v>
       </c>
       <c r="D31" t="n">
-        <v>106.9965576648151</v>
+        <v>150.6996278309037</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.06770766429676045</v>
+        <v>0.09185435055834401</v>
       </c>
       <c r="G31" t="n">
-        <v>0.07023450989472069</v>
+        <v>0.09427511040186254</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>4040</v>
+        <v>2594</v>
       </c>
       <c r="B32" t="n">
-        <v>0.2666341245317104</v>
+        <v>0.2860839662074056</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0006944713171908174</v>
+        <v>0.001099655719688007</v>
       </c>
       <c r="D32" t="n">
-        <v>-22.64085302333649</v>
+        <v>-18.36247688598045</v>
       </c>
       <c r="E32" t="n">
-        <v>2.612385498842137e-113</v>
+        <v>2.721810149556562e-75</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.01708457230030521</v>
+        <v>-0.0223476916943383</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.01436227374257519</v>
+        <v>-0.01803711377627615</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>4041</v>
+        <v>2828</v>
       </c>
       <c r="B33" t="n">
-        <v>0.3393275636749906</v>
+        <v>0.366588257431141</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0006458409675708682</v>
+        <v>0.0006213314969083186</v>
       </c>
       <c r="D33" t="n">
-        <v>88.21059515025061</v>
+        <v>97.06877695486858</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.05570418131266958</v>
+        <v>0.05909409923747546</v>
       </c>
       <c r="G33" t="n">
-        <v>0.05823585093101041</v>
+        <v>0.06152967773938093</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>4050</v>
+        <v>2830</v>
       </c>
       <c r="B34" t="n">
-        <v>0.3539945756573217</v>
+        <v>0.368356818550918</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0006577932975236524</v>
+        <v>0.0006195067743694569</v>
       </c>
       <c r="D34" t="n">
-        <v>108.9050745482782</v>
+        <v>100.2094765975587</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.07034776697789691</v>
+        <v>0.06086623675327431</v>
       </c>
       <c r="G34" t="n">
-        <v>0.07292628923044531</v>
+        <v>0.06329466246313606</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>4054</v>
+        <v>2832</v>
       </c>
       <c r="B35" t="n">
-        <v>0.3493057441310997</v>
+        <v>0.349653281469202</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0006881793705597249</v>
+        <v>0.0006191797067007961</v>
       </c>
       <c r="D35" t="n">
-        <v>97.28306229740271</v>
+        <v>70.05544926143727</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.06559937938308463</v>
+        <v>0.04216334071340672</v>
       </c>
       <c r="G35" t="n">
-        <v>0.06829701377281355</v>
+        <v>0.04459048433957174</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>4057</v>
+        <v>2835</v>
       </c>
       <c r="B36" t="n">
-        <v>0.3127130529850591</v>
+        <v>0.3860667584326041</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0006765385041308921</v>
+        <v>0.0006509696260943366</v>
       </c>
       <c r="D36" t="n">
-        <v>44.86885113938103</v>
+        <v>122.5716013335595</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.02902950409214526</v>
+        <v>0.07851451048279282</v>
       </c>
       <c r="G36" t="n">
-        <v>0.03168150677167177</v>
+        <v>0.08106626849698981</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>4072</v>
+        <v>2836</v>
       </c>
       <c r="B37" t="n">
-        <v>0.3105424046907229</v>
+        <v>0.3265251814657868</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0007154737741058643</v>
+        <v>0.00061893184831086</v>
       </c>
       <c r="D37" t="n">
-        <v>39.39327779385789</v>
+        <v>32.71573853944574</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1.348542076449828e-234</v>
       </c>
       <c r="F37" t="n">
-        <v>0.02678254348175363</v>
+        <v>0.01903572650426479</v>
       </c>
       <c r="G37" t="n">
-        <v>0.02958717079339085</v>
+        <v>0.02146189854188319</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>4078</v>
+        <v>2837</v>
       </c>
       <c r="B38" t="n">
-        <v>0.3293340520462328</v>
+        <v>0.3784296342905815</v>
       </c>
       <c r="C38" t="n">
-        <v>0.000764019407967132</v>
+        <v>0.0006103965506036834</v>
       </c>
       <c r="D38" t="n">
-        <v>61.48600939088073</v>
+        <v>118.2071970696901</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.04547904240868689</v>
+        <v>0.0709569082311885</v>
       </c>
       <c r="G38" t="n">
-        <v>0.04847396657747755</v>
+        <v>0.07334962246454879</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>4271</v>
+        <v>2838</v>
       </c>
       <c r="B39" t="n">
-        <v>0.2780970454648892</v>
+        <v>0.2366740238227227</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0007254742829528604</v>
+        <v>0.00123964197047848</v>
       </c>
       <c r="D39" t="n">
-        <v>-5.872712773387495</v>
+        <v>-56.14713504184186</v>
       </c>
       <c r="E39" t="n">
-        <v>4.295814664097004e-09</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.005682416532576841</v>
+        <v>-0.07203200251574474</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.002838587643945953</v>
+        <v>-0.06717268772423557</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>6017</v>
+        <v>2840</v>
       </c>
       <c r="B40" t="n">
-        <v>0.338395242920467</v>
+        <v>0.3862696330162169</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0006517785027931305</v>
+        <v>0.0006238920147395766</v>
       </c>
       <c r="D40" t="n">
-        <v>85.97659347028554</v>
+        <v>128.2165217435819</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.05476022311310542</v>
+        <v>0.07877045629201281</v>
       </c>
       <c r="G40" t="n">
-        <v>0.05731516762152727</v>
+        <v>0.08121607185499531</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>3399</v>
+        <v>2843</v>
       </c>
       <c r="B41" t="n">
-        <v>0.2823575475531506</v>
-      </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
+        <v>0.3169508537191817</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.0006533573124044148</v>
+      </c>
+      <c r="D41" t="n">
+        <v>16.33789746254749</v>
+      </c>
+      <c r="E41" t="n">
+        <v>5.428860550512845e-60</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.009393925982915826</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.01195504357002205</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2843</v>
+        <v>2850</v>
       </c>
       <c r="B42" t="n">
-        <v>0.3175664369150925</v>
+        <v>0.3544358876250185</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0005641684014629425</v>
+        <v>0.000610817904319336</v>
       </c>
       <c r="D42" t="n">
-        <v>-110.0443393378028</v>
+        <v>78.84431406111476</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.06318929719232669</v>
+        <v>0.04696233572623332</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.06097778083618094</v>
+        <v>0.04935670163837803</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2850</v>
+        <v>2857</v>
       </c>
       <c r="B43" t="n">
-        <v>0.358328692409994</v>
+        <v>0.2970532846923992</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0005627878422473868</v>
+        <v>0.002001803462164073</v>
       </c>
       <c r="D43" t="n">
-        <v>-37.88511747910135</v>
+        <v>-4.607387500640495</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>4.0782420253048e-06</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.02242433583045529</v>
+        <v>-0.01314655304414347</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.02021823120824912</v>
+        <v>-0.005299615456483768</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2857</v>
+        <v>2861</v>
       </c>
       <c r="B44" t="n">
-        <v>0.2815501964227486</v>
+        <v>0.3466402833672715</v>
       </c>
       <c r="C44" t="n">
-        <v>0.001655598200154015</v>
+        <v>0.0006289201362254359</v>
       </c>
       <c r="D44" t="n">
-        <v>-59.2533740961253</v>
+        <v>64.17971392490165</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.1013447170902621</v>
+        <v>0.03913125169071357</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.09485484192293307</v>
+        <v>0.04159657715840374</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2861</v>
+        <v>2864</v>
       </c>
       <c r="B45" t="n">
-        <v>0.350919715010892</v>
+        <v>0.07498403782092947</v>
       </c>
       <c r="C45" t="n">
-        <v>0.000558020921458388</v>
+        <v>0.0006482703169493599</v>
       </c>
       <c r="D45" t="n">
-        <v>-51.48599239499418</v>
+        <v>-356.7837753395871</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.0298239701652648</v>
+        <v>-0.2325629195719439</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.02763655167164361</v>
+        <v>-0.2300217426716228</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2864</v>
+        <v>2866</v>
       </c>
       <c r="B46" t="n">
-        <v>0.05446556197329949</v>
+        <v>0.3443957725059817</v>
       </c>
       <c r="C46" t="n">
-        <v>0.0005767965813151867</v>
+        <v>0.0006153626574068595</v>
       </c>
       <c r="D46" t="n">
-        <v>-563.7765973136929</v>
+        <v>61.94624113836259</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>-0.3263149231005147</v>
+        <v>0.03691331304096862</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.3240539048115788</v>
+        <v>0.03932549408556923</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2866</v>
+        <v>2872</v>
       </c>
       <c r="B47" t="n">
-        <v>0.3477325284889476</v>
+        <v>0.3738911562117907</v>
       </c>
       <c r="C47" t="n">
-        <v>0.0005331867721217394</v>
+        <v>0.0006105797553085082</v>
       </c>
       <c r="D47" t="n">
-        <v>-59.86166407202451</v>
+        <v>110.7386654752648</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.03296248227784269</v>
+        <v>0.06641807107721588</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.03087241260295461</v>
+        <v>0.06881150346093994</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2872</v>
+        <v>2876</v>
       </c>
       <c r="B48" t="n">
-        <v>0.3782338218995807</v>
+        <v>0.3728291968517204</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0005574918059815563</v>
+        <v>0.0006178528107784788</v>
       </c>
       <c r="D48" t="n">
-        <v>-2.54022393615671</v>
+        <v>107.7163148698033</v>
       </c>
       <c r="E48" t="n">
-        <v>0.01107909555988421</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.002508826221391707</v>
+        <v>0.06534185676819002</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.000323481838139457</v>
+        <v>0.06776379904982519</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2876</v>
+        <v>2878</v>
       </c>
       <c r="B49" t="n">
-        <v>0.3733548775507737</v>
+        <v>0.3626823737232957</v>
       </c>
       <c r="C49" t="n">
-        <v>0.0006049922315637218</v>
+        <v>0.0006104893397596888</v>
       </c>
       <c r="D49" t="n">
-        <v>-10.40525489443324</v>
+        <v>92.39474157367989</v>
       </c>
       <c r="E49" t="n">
-        <v>2.390775889880699e-25</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.007480870403356996</v>
+        <v>0.05520946580021591</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.005109326353788015</v>
+        <v>0.05760254376094991</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2878</v>
+        <v>3113</v>
       </c>
       <c r="B50" t="n">
-        <v>0.366919959144779</v>
+        <v>0.3645629788591395</v>
       </c>
       <c r="C50" t="n">
-        <v>0.0005488107306633316</v>
+        <v>0.0006147860550174422</v>
       </c>
       <c r="D50" t="n">
-        <v>-23.1956411806687</v>
+        <v>94.80795707829287</v>
       </c>
       <c r="E50" t="n">
-        <v>7.953739288012723e-119</v>
+        <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.0138056742515071</v>
+        <v>0.05708164951580118</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.01165435931762742</v>
+        <v>0.05949157031705214</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>3113</v>
+        <v>3118</v>
       </c>
       <c r="B51" t="n">
-        <v>0.3635879181339076</v>
+        <v>0.3594491715568007</v>
       </c>
       <c r="C51" t="n">
-        <v>0.0005245297635276309</v>
+        <v>0.0006163771769232627</v>
       </c>
       <c r="D51" t="n">
-        <v>-30.6218234164944</v>
+        <v>86.26666366770388</v>
       </c>
       <c r="E51" t="n">
-        <v>2.497840601797455e-205</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>-0.01709012507846854</v>
+        <v>0.0519647236669804</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.01503399051240882</v>
+        <v>0.05438088156119544</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>3118</v>
+        <v>3131</v>
       </c>
       <c r="B52" t="n">
-        <v>0.3621463944344837</v>
+        <v>0.3532537587841877</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0005811938249897991</v>
+        <v>0.0006088288590019383</v>
       </c>
       <c r="D52" t="n">
-        <v>-30.11659921742931</v>
+        <v>77.16025471999737</v>
       </c>
       <c r="E52" t="n">
-        <v>1.070870945095824e-198</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>-0.01864270914426907</v>
+        <v>0.04578410534865324</v>
       </c>
       <c r="G52" t="n">
-        <v>-0.01636445384545599</v>
+        <v>0.04817067433429661</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>3131</v>
+        <v>3140</v>
       </c>
       <c r="B53" t="n">
-        <v>0.3565012520393566</v>
+        <v>0.3569949502459204</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0005597642882772047</v>
+        <v>0.0006099888736126329</v>
       </c>
       <c r="D53" t="n">
-        <v>-41.35441358939637</v>
+        <v>83.14673184582695</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>-0.0242458500990269</v>
+        <v>0.04952302321999033</v>
       </c>
       <c r="G53" t="n">
-        <v>-0.02205159768095234</v>
+        <v>0.05191413938642489</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>3140</v>
+        <v>3148</v>
       </c>
       <c r="B54" t="n">
-        <v>0.3595794845981934</v>
+        <v>0.3489625878078281</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0005440682624191079</v>
+        <v>0.0006385785473187161</v>
       </c>
       <c r="D54" t="n">
-        <v>-36.88965653301075</v>
+        <v>66.84568256222751</v>
       </c>
       <c r="E54" t="n">
-        <v>1.235166301679413e-296</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>-0.02113685366027267</v>
+        <v>0.04143462596392923</v>
       </c>
       <c r="G54" t="n">
-        <v>-0.01900412900203304</v>
+        <v>0.04393781176630131</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>3148</v>
+        <v>3152</v>
       </c>
       <c r="B55" t="n">
-        <v>0.332807742144667</v>
+        <v>0.07498403782092278</v>
       </c>
       <c r="C55" t="n">
-        <v>0.0005457134650608027</v>
+        <v>0.0006444326010613946</v>
       </c>
       <c r="D55" t="n">
-        <v>-85.83668313821086</v>
+        <v>-358.9084890194048</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>-0.04791182067630718</v>
+        <v>-0.2325553977753254</v>
       </c>
       <c r="G55" t="n">
-        <v>-0.04577264689305126</v>
+        <v>-0.2300292644682547</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>3152</v>
+        <v>3178</v>
       </c>
       <c r="B56" t="n">
-        <v>0.05536646969903547</v>
+        <v>0.3320456453850303</v>
       </c>
       <c r="C56" t="n">
-        <v>0.0005819185149157248</v>
+        <v>0.0006354181960016357</v>
       </c>
       <c r="D56" t="n">
-        <v>-557.2661771679055</v>
+        <v>40.55482925177538</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>-0.3254240542567006</v>
+        <v>0.0245238777255279</v>
       </c>
       <c r="G56" t="n">
-        <v>-0.3231429582039209</v>
+        <v>0.02701467515910706</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3178</v>
+        <v>3179</v>
       </c>
       <c r="B57" t="n">
-        <v>0.3384898220472556</v>
+        <v>0.3548932417259343</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0007115531763930493</v>
+        <v>0.0006114901026966637</v>
       </c>
       <c r="D57" t="n">
-        <v>-57.84550648868795</v>
+        <v>79.50557591827196</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>-0.0425547831131679</v>
+        <v>0.04741837234048947</v>
       </c>
       <c r="G57" t="n">
-        <v>-0.03976552465101341</v>
+        <v>0.04981537322595354</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>3179</v>
+        <v>3181</v>
       </c>
       <c r="B58" t="n">
-        <v>0.3591220214764339</v>
+        <v>0.3181468009814968</v>
       </c>
       <c r="C58" t="n">
-        <v>0.0005584335996378978</v>
+        <v>0.0007276475871051489</v>
       </c>
       <c r="D58" t="n">
-        <v>-36.75988419433076</v>
+        <v>16.31343558220127</v>
       </c>
       <c r="E58" t="n">
-        <v>1.416074327475086e-294</v>
+        <v>8.104632596772996e-60</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.0216224725402584</v>
+        <v>0.01044426675589142</v>
       </c>
       <c r="G58" t="n">
-        <v>-0.01943343636556637</v>
+        <v>0.01329659732167665</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>3181</v>
+        <v>3393</v>
       </c>
       <c r="B59" t="n">
-        <v>0.3208061795839359</v>
+        <v>0.4585894767002988</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0006224325544868234</v>
+        <v>0.0006213243982199897</v>
       </c>
       <c r="D59" t="n">
-        <v>-94.53842978043666</v>
+        <v>245.1426472128609</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>-0.06006375103560194</v>
+        <v>0.1510953324198284</v>
       </c>
       <c r="G59" t="n">
-        <v>-0.0576238416552188</v>
+        <v>0.1535308830953437</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>3393</v>
+        <v>3399</v>
       </c>
       <c r="B60" t="n">
-        <v>0.4609577590097755</v>
+        <v>0.2875138306025535</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0005336476758499001</v>
+        <v>0.0006219188568910118</v>
       </c>
       <c r="D60" t="n">
-        <v>152.3622921264231</v>
+        <v>-30.16878831099236</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>7.940650016817877e-200</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0802618448813907</v>
+        <v>-0.01998147879731502</v>
       </c>
       <c r="G60" t="n">
-        <v>0.08235372127946779</v>
+        <v>-0.01754359788300355</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2840</v>
+        <v>3403</v>
       </c>
       <c r="B61" t="n">
-        <v>0.3796499759293462</v>
-      </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+        <v>0.3794174081037961</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.0006143923329100722</v>
+      </c>
+      <c r="D61" t="n">
+        <v>119.0461456682742</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.07193685044280866</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.07434522787935784</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2107</v>
+        <v>3406</v>
       </c>
       <c r="B62" t="n">
-        <v>0.3302673384856623</v>
+        <v>0.3625039287412528</v>
       </c>
       <c r="C62" t="n">
-        <v>0.0007098303195501771</v>
+        <v>0.0006174807946754915</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.5393354652913575</v>
+        <v>91.05960911397992</v>
       </c>
       <c r="E62" t="n">
-        <v>0.5896561866942949</v>
+        <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>-0.001774089535677325</v>
+        <v>0.05501731779702024</v>
       </c>
       <c r="G62" t="n">
-        <v>0.001008416204332309</v>
+        <v>0.05743780180005967</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2161</v>
+        <v>3942</v>
       </c>
       <c r="B63" t="n">
-        <v>0.3319557682035102</v>
+        <v>0.3285665416336612</v>
       </c>
       <c r="C63" t="n">
-        <v>0.0006849399887107081</v>
+        <v>0.0006388663888391639</v>
       </c>
       <c r="D63" t="n">
-        <v>1.906142251429939</v>
+        <v>34.89019469540436</v>
       </c>
       <c r="E63" t="n">
-        <v>0.0566336244564291</v>
+        <v>1.686138071778233e-266</v>
       </c>
       <c r="F63" t="n">
-        <v>-3.687527980384547e-05</v>
+        <v>0.02103801562987128</v>
       </c>
       <c r="G63" t="n">
-        <v>0.002648061384154698</v>
+        <v>0.02354232975202538</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2167</v>
+        <v>3943</v>
       </c>
       <c r="B64" t="n">
-        <v>0.3300734088978481</v>
+        <v>0.3521738268264451</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0007260764796372963</v>
+        <v>0.0006150933101437681</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.7943601943625213</v>
+        <v>74.61869138684747</v>
       </c>
       <c r="E64" t="n">
-        <v>0.4269870028241797</v>
+        <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>-0.001999861264106351</v>
+        <v>0.04469189527318827</v>
       </c>
       <c r="G64" t="n">
-        <v>0.0008463287571328752</v>
+        <v>0.04710302049427631</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2168</v>
+        <v>3944</v>
       </c>
       <c r="B65" t="n">
-        <v>0.3362366685440576</v>
+        <v>0.3387452136529148</v>
       </c>
       <c r="C65" t="n">
-        <v>0.000756318495989801</v>
+        <v>0.0006099569351606194</v>
       </c>
       <c r="D65" t="n">
-        <v>7.38642968847632</v>
+        <v>53.23137231262403</v>
       </c>
       <c r="E65" t="n">
-        <v>1.51586033371029e-13</v>
+        <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>0.004104124650217798</v>
+        <v>0.03127334922529779</v>
       </c>
       <c r="G65" t="n">
-        <v>0.007068862135227851</v>
+        <v>0.03366434019510623</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2364</v>
+        <v>3945</v>
       </c>
       <c r="B66" t="n">
-        <v>0.355255120123338</v>
+        <v>0.2974091355396906</v>
       </c>
       <c r="C66" t="n">
-        <v>0.0007322729777006689</v>
+        <v>0.0009914184382938558</v>
       </c>
       <c r="D66" t="n">
-        <v>33.60078238754971</v>
+        <v>-8.943986777451835</v>
       </c>
       <c r="E66" t="n">
-        <v>1.303653043612691e-246</v>
+        <v>3.761693355523482e-19</v>
       </c>
       <c r="F66" t="n">
-        <v>0.02316970495224943</v>
+        <v>-0.01081038085870116</v>
       </c>
       <c r="G66" t="n">
-        <v>0.026040184991757</v>
+        <v>-0.006924085947343225</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2378</v>
+        <v>3946</v>
       </c>
       <c r="B67" t="n">
-        <v>0.3291826076144387</v>
+        <v>0.3168760757565139</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0007148074372698239</v>
+        <v>0.0007408039465486158</v>
       </c>
       <c r="D67" t="n">
-        <v>-2.05309494610388</v>
+        <v>14.30838329518196</v>
       </c>
       <c r="E67" t="n">
-        <v>0.04006506690702051</v>
+        <v>1.966258005793977e-46</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.002868575455566953</v>
+        <v>0.009147755500115495</v>
       </c>
       <c r="G67" t="n">
-        <v>-6.655961822532998e-05</v>
+        <v>0.01205165812748668</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2516</v>
+        <v>3947</v>
       </c>
       <c r="B68" t="n">
-        <v>0.3465160739472578</v>
+        <v>0.3906734172668431</v>
       </c>
       <c r="C68" t="n">
-        <v>0.0006781549749896293</v>
+        <v>0.0006135350848986792</v>
       </c>
       <c r="D68" t="n">
-        <v>23.39568296489399</v>
+        <v>137.5586342190485</v>
       </c>
       <c r="E68" t="n">
-        <v>7.720808770346423e-121</v>
+        <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>0.01453672895169844</v>
+        <v>0.08319453978369774</v>
       </c>
       <c r="G68" t="n">
-        <v>0.01719506864014753</v>
+        <v>0.08559955686456282</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2517</v>
+        <v>3948</v>
       </c>
       <c r="B69" t="n">
-        <v>0.3584924973516838</v>
+        <v>0.3720184512351761</v>
       </c>
       <c r="C69" t="n">
-        <v>0.0006791544220763363</v>
+        <v>0.0006117448855608389</v>
       </c>
       <c r="D69" t="n">
-        <v>40.99556933639393</v>
+        <v>107.4665008963531</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>0.02651119346032991</v>
+        <v>0.06454308248371673</v>
       </c>
       <c r="G69" t="n">
-        <v>0.02917345094036807</v>
+        <v>0.06694108210120989</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2527</v>
+        <v>3954</v>
       </c>
       <c r="B70" t="n">
-        <v>0.3438101691048976</v>
+        <v>0.3548520621909371</v>
       </c>
       <c r="C70" t="n">
-        <v>0.0007411353203960644</v>
+        <v>0.00062067090175065</v>
       </c>
       <c r="D70" t="n">
-        <v>17.75653324217504</v>
+        <v>78.26320375453844</v>
       </c>
       <c r="E70" t="n">
-        <v>1.806346338173555e-70</v>
+        <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>0.01170738392386386</v>
+        <v>0.04735919874200316</v>
       </c>
       <c r="G70" t="n">
-        <v>0.01461260398326167</v>
+        <v>0.0497921877544453</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2535</v>
+        <v>4040</v>
       </c>
       <c r="B71" t="n">
-        <v>0.31522687336074</v>
+        <v>0.2812610314590914</v>
       </c>
       <c r="C71" t="n">
-        <v>0.0007284439389431682</v>
+        <v>0.0006476346110012312</v>
       </c>
       <c r="D71" t="n">
-        <v>-21.17294271535988</v>
+        <v>-38.62569581472521</v>
       </c>
       <c r="E71" t="n">
-        <v>2.357761738578738e-99</v>
+        <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>-0.01685103697290504</v>
+        <v>-0.02628467997108049</v>
       </c>
       <c r="G71" t="n">
-        <v>-0.01399556660828459</v>
+        <v>-0.02374599499616241</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2554</v>
+        <v>4041</v>
       </c>
       <c r="B72" t="n">
-        <v>0.3932930843595144</v>
+        <v>0.3476871133356313</v>
       </c>
       <c r="C72" t="n">
-        <v>0.0006978358114764537</v>
+        <v>0.0006109793148905918</v>
       </c>
       <c r="D72" t="n">
-        <v>89.7674039909791</v>
+        <v>67.7776536515544</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>0.06127516532803085</v>
+        <v>0.04021324507744761</v>
       </c>
       <c r="G72" t="n">
-        <v>0.06401065308832826</v>
+        <v>0.04260824370838943</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2594</v>
+        <v>4050</v>
       </c>
       <c r="B73" t="n">
-        <v>0.2882393600782763</v>
+        <v>0.36671709223014</v>
       </c>
       <c r="C73" t="n">
-        <v>0.001150193729402288</v>
+        <v>0.0006243052432466776</v>
       </c>
       <c r="D73" t="n">
-        <v>-36.87275803102995</v>
+        <v>96.81277538709635</v>
       </c>
       <c r="E73" t="n">
-        <v>2.556970589909758e-296</v>
+        <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.04466517119595073</v>
+        <v>0.05921710559168459</v>
       </c>
       <c r="G73" t="n">
-        <v>-0.04015645895016631</v>
+        <v>0.06166434098316972</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2828</v>
+        <v>4054</v>
       </c>
       <c r="B74" t="n">
-        <v>0.361010244156995</v>
+        <v>0.355233842901103</v>
       </c>
       <c r="C74" t="n">
-        <v>0.0006911936430395243</v>
+        <v>0.0006242724032458185</v>
       </c>
       <c r="D74" t="n">
-        <v>43.92411491539733</v>
+        <v>78.42325514285527</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.02900534363943856</v>
+        <v>0.04773392062796676</v>
       </c>
       <c r="G74" t="n">
-        <v>0.03171479437188181</v>
+        <v>0.05018102728881375</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2830</v>
+        <v>4057</v>
       </c>
       <c r="B75" t="n">
-        <v>0.3617752352609503</v>
+        <v>0.3252532731864814</v>
       </c>
       <c r="C75" t="n">
-        <v>0.0006964023648213903</v>
+        <v>0.0006310773011558038</v>
       </c>
       <c r="D75" t="n">
-        <v>44.69407584162679</v>
+        <v>30.0706493626261</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>1.52584305255884e-198</v>
       </c>
       <c r="F75" t="n">
-        <v>0.02976012575551535</v>
+        <v>0.01774001353777367</v>
       </c>
       <c r="G75" t="n">
-        <v>0.03248999446371558</v>
+        <v>0.02021379494976347</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2832</v>
+        <v>4072</v>
       </c>
       <c r="B76" t="n">
-        <v>0.3420629151497215</v>
+        <v>0.3119231339086644</v>
       </c>
       <c r="C76" t="n">
-        <v>0.0007001983150130422</v>
+        <v>0.0006114731740527353</v>
       </c>
       <c r="D76" t="n">
-        <v>16.29929657596239</v>
+        <v>9.234689607928107</v>
       </c>
       <c r="E76" t="n">
-        <v>1.121231482939529e-59</v>
+        <v>2.596561151358604e-20</v>
       </c>
       <c r="F76" t="n">
-        <v>0.01004036565975356</v>
+        <v>0.004448297702803594</v>
       </c>
       <c r="G76" t="n">
-        <v>0.01278511433701986</v>
+        <v>0.006845232229099624</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2835</v>
+        <v>4078</v>
       </c>
       <c r="B77" t="n">
-        <v>0.3784464285523699</v>
+        <v>0.3404570467202485</v>
       </c>
       <c r="C77" t="n">
-        <v>0.0009551294942939644</v>
+        <v>0.0006292556524004957</v>
       </c>
       <c r="D77" t="n">
-        <v>50.04164742746877</v>
+        <v>54.31922247681469</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>0.04592421917882153</v>
+        <v>0.03294735744304821</v>
       </c>
       <c r="G77" t="n">
-        <v>0.04966828762324868</v>
+        <v>0.03541399811202318</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2836</v>
+        <v>4271</v>
       </c>
       <c r="B78" t="n">
-        <v>0.3189576723806348</v>
+        <v>0.2841541883009748</v>
       </c>
       <c r="C78" t="n">
-        <v>0.0007054824150098801</v>
+        <v>0.0006863646726424798</v>
       </c>
       <c r="D78" t="n">
-        <v>-16.57376927040244</v>
+        <v>-32.23094300085177</v>
       </c>
       <c r="E78" t="n">
-        <v>1.220943768829071e-61</v>
+        <v>9.207465820072503e-228</v>
       </c>
       <c r="F78" t="n">
-        <v>-0.01307523383696728</v>
+        <v>-0.02346743277322792</v>
       </c>
       <c r="G78" t="n">
-        <v>-0.01030977170443282</v>
+        <v>-0.02077692851024818</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2837</v>
+        <v>6017</v>
       </c>
       <c r="B79" t="n">
-        <v>0.3734894828902878</v>
+        <v>0.3471029659768197</v>
       </c>
       <c r="C79" t="n">
-        <v>0.0007227514007227219</v>
+        <v>0.0006136253243235076</v>
       </c>
       <c r="D79" t="n">
-        <v>59.2725350599327</v>
+        <v>66.53342913954242</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>0.04142272981481939</v>
+        <v>0.0396239116273765</v>
       </c>
       <c r="G79" t="n">
-        <v>0.04425588566308662</v>
+        <v>0.04202928244083717</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2838</v>
+        <v>6018</v>
       </c>
       <c r="B80" t="n">
-        <v>0.2376319738304558</v>
+        <v>0.3315516142654211</v>
       </c>
       <c r="C80" t="n">
-        <v>0.00129009910151337</v>
+        <v>0.0006384013021196542</v>
       </c>
       <c r="D80" t="n">
-        <v>-72.10159375490043</v>
+        <v>39.59146893777955</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>-0.0955467691041044</v>
+        <v>0.02402399981626932</v>
       </c>
       <c r="G80" t="n">
-        <v>-0.09048963353765374</v>
+        <v>0.0265264908291473</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2104</v>
+        <v>6025</v>
       </c>
       <c r="B81" t="n">
-        <v>0.3306501751513348</v>
-      </c>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr"/>
+        <v>0.1805439184142131</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.000638205180603868</v>
+      </c>
+      <c r="D81" t="n">
+        <v>-197.0094482929958</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-0.1269833116432332</v>
+      </c>
+      <c r="G81" t="n">
+        <v>-0.1244815894137663</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1382</v>
+        <v>6041</v>
       </c>
       <c r="B82" t="n">
-        <v>0.3071036825719191</v>
+        <v>0.3591488135711853</v>
       </c>
       <c r="C82" t="n">
-        <v>0.0005212623576533621</v>
+        <v>0.0006546395985097162</v>
       </c>
       <c r="D82" t="n">
-        <v>-68.12086368194333</v>
+        <v>80.76572933998554</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>-0.03653050497369318</v>
+        <v>0.05158937259642524</v>
       </c>
       <c r="G82" t="n">
-        <v>-0.03448717904277297</v>
+        <v>0.05415551666051984</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1384</v>
+        <v>6052</v>
       </c>
       <c r="B83" t="n">
-        <v>0.3674506432306689</v>
+        <v>0.3848130150683902</v>
       </c>
       <c r="C83" t="n">
-        <v>0.0005282200673878048</v>
+        <v>0.0006120002451224833</v>
       </c>
       <c r="D83" t="n">
-        <v>47.0222927601901</v>
+        <v>128.3278017477908</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>0.02380281872421388</v>
+        <v>0.07733714582060827</v>
       </c>
       <c r="G83" t="n">
-        <v>0.02587341857681952</v>
+        <v>0.07973614643074656</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1552</v>
+        <v>6061</v>
       </c>
       <c r="B84" t="n">
-        <v>0.3175238917738089</v>
+        <v>0.3010952388875507</v>
       </c>
       <c r="C84" t="n">
-        <v>0.0005227474162999297</v>
+        <v>0.0006116995313232744</v>
       </c>
       <c r="D84" t="n">
-        <v>-47.99379590228047</v>
+        <v>-8.470057258265113</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>2.456896573659513e-17</v>
       </c>
       <c r="F84" t="n">
-        <v>-0.026113206454684</v>
+        <v>-0.006380040971098181</v>
       </c>
       <c r="G84" t="n">
-        <v>-0.02406405915800254</v>
+        <v>-0.003982219139225954</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1570</v>
+        <v>6073</v>
       </c>
       <c r="B85" t="n">
-        <v>0.313144789459593</v>
+        <v>0.3283061676036159</v>
       </c>
       <c r="C85" t="n">
-        <v>0.0006613111076617524</v>
+        <v>0.0006668994974478404</v>
       </c>
       <c r="D85" t="n">
-        <v>-44.5595647482022</v>
+        <v>33.03316128623424</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>3.98167473494626e-239</v>
       </c>
       <c r="F85" t="n">
-        <v>-0.03076389061198391</v>
+        <v>0.0207226976311003</v>
       </c>
       <c r="G85" t="n">
-        <v>-0.02817157962913443</v>
+        <v>0.02333689969070584</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1571</v>
+        <v>6090</v>
       </c>
       <c r="B86" t="n">
-        <v>0.3972735822360505</v>
+        <v>0.3199191849779457</v>
       </c>
       <c r="C86" t="n">
-        <v>0.0005875257304146527</v>
+        <v>0.0006147409265606862</v>
       </c>
       <c r="D86" t="n">
-        <v>93.03602349010427</v>
+        <v>22.19278958952815</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>4.360002622377647e-109</v>
       </c>
       <c r="F86" t="n">
-        <v>0.0535095199106412</v>
+        <v>0.01243794408489493</v>
       </c>
       <c r="G86" t="n">
-        <v>0.05581259540115539</v>
+        <v>0.01484768798557084</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1573</v>
+        <v>6094</v>
       </c>
       <c r="B87" t="n">
-        <v>0.3671298937753824</v>
+        <v>0.3888636906135279</v>
       </c>
       <c r="C87" t="n">
-        <v>0.0005343417619653556</v>
+        <v>0.0006194046189631582</v>
       </c>
       <c r="D87" t="n">
-        <v>45.88331090771047</v>
+        <v>133.3333965269111</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>0.02347007087974025</v>
+        <v>0.08137330903711285</v>
       </c>
       <c r="G87" t="n">
-        <v>0.02556466751072022</v>
+        <v>0.08380133430451728</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1606</v>
+        <v>6101</v>
       </c>
       <c r="B88" t="n">
-        <v>0.335313234179113</v>
+        <v>0.2711453212372895</v>
       </c>
       <c r="C88" t="n">
-        <v>0.0008135219311339244</v>
+        <v>0.0007062564382942321</v>
       </c>
       <c r="D88" t="n">
-        <v>-8.972456822233578</v>
+        <v>-49.7426229349112</v>
       </c>
       <c r="E88" t="n">
-        <v>2.929138093892798e-19</v>
+        <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>-0.008893775819803766</v>
+        <v>-0.03651528704183317</v>
       </c>
       <c r="G88" t="n">
-        <v>-0.005704804982274666</v>
+        <v>-0.03374680836901357</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1619</v>
+        <v>6113</v>
       </c>
       <c r="B89" t="n">
-        <v>0.4044770005983881</v>
+        <v>0.3953300485021636</v>
       </c>
       <c r="C89" t="n">
-        <v>0.000641642998174722</v>
+        <v>0.0006113325441438247</v>
       </c>
       <c r="D89" t="n">
-        <v>96.41572680481423</v>
+        <v>145.6714196103711</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>0.06060686959671519</v>
+        <v>0.08785548792628819</v>
       </c>
       <c r="G89" t="n">
-        <v>0.06312208243975664</v>
+        <v>0.09025187119261338</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1702</v>
+        <v>6124</v>
       </c>
       <c r="B90" t="n">
-        <v>0.4153366295028668</v>
+        <v>0.4039347822646063</v>
       </c>
       <c r="C90" t="n">
-        <v>0.0005858693351743716</v>
+        <v>0.0007105185743386222</v>
       </c>
       <c r="D90" t="n">
-        <v>124.1302463817633</v>
+        <v>137.4466718379568</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>0.07157581367636215</v>
+        <v>0.09626582033934344</v>
       </c>
       <c r="G90" t="n">
-        <v>0.07387239616906702</v>
+        <v>0.09905100630444352</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1710</v>
+        <v>6155</v>
       </c>
       <c r="B91" t="n">
-        <v>0.3744980679520208</v>
+        <v>0.3316487983185754</v>
       </c>
       <c r="C91" t="n">
-        <v>0.0005301649302211287</v>
+        <v>0.0006112048803131438</v>
       </c>
       <c r="D91" t="n">
-        <v>60.14268684005435</v>
+        <v>41.51215115112178</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>0.0308464315564076</v>
+        <v>0.02417448795959946</v>
       </c>
       <c r="G91" t="n">
-        <v>0.03292465518732961</v>
+        <v>0.02657037079212558</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1720</v>
+        <v>6195</v>
       </c>
       <c r="B92" t="n">
-        <v>0.3652247412721238</v>
+        <v>0.3618702336204086</v>
       </c>
       <c r="C92" t="n">
-        <v>0.0005661863808670366</v>
+        <v>0.0006367307167643795</v>
       </c>
       <c r="D92" t="n">
-        <v>39.93776158540604</v>
+        <v>87.31142257468339</v>
       </c>
       <c r="E92" t="n">
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>0.02150250361105045</v>
+        <v>0.05434589346348014</v>
       </c>
       <c r="G92" t="n">
-        <v>0.02372192977289277</v>
+        <v>0.05684183589191141</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1723</v>
+        <v>6639</v>
       </c>
       <c r="B93" t="n">
-        <v>0.368045908020509</v>
+        <v>0.3271867382902052</v>
       </c>
       <c r="C93" t="n">
-        <v>0.0005473086970853368</v>
+        <v>0.0006363596055771369</v>
       </c>
       <c r="D93" t="n">
-        <v>46.4699055136543</v>
+        <v>32.85935996601797</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>1.218147476972269e-236</v>
       </c>
       <c r="F93" t="n">
-        <v>0.02436067021202479</v>
+        <v>0.01966312549896957</v>
       </c>
       <c r="G93" t="n">
-        <v>0.02650609666868889</v>
+        <v>0.02215761319601515</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1912</v>
+        <v>6705</v>
       </c>
       <c r="B94" t="n">
-        <v>0.2775339977937848</v>
+        <v>0.2992432284895948</v>
       </c>
       <c r="C94" t="n">
-        <v>0.0005449881632156771</v>
+        <v>0.0007830429652366952</v>
       </c>
       <c r="D94" t="n">
-        <v>-119.4127344021098</v>
+        <v>-8.981806574294502</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>2.669281060819434e-19</v>
       </c>
       <c r="F94" t="n">
-        <v>-0.06614669181842178</v>
+        <v>-0.008567878850968956</v>
       </c>
       <c r="G94" t="n">
-        <v>-0.06401036175431288</v>
+        <v>-0.005498402055267064</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2049</v>
+        <v>8002</v>
       </c>
       <c r="B95" t="n">
-        <v>0.365945685093688</v>
+        <v>0.2661755492430334</v>
       </c>
       <c r="C95" t="n">
-        <v>0.000538677455783756</v>
+        <v>0.001079456619784992</v>
       </c>
       <c r="D95" t="n">
-        <v>43.3156432722564</v>
+        <v>-37.14907942078002</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>8.367499959021055e-302</v>
       </c>
       <c r="F95" t="n">
-        <v>0.02227736433178179</v>
+        <v>-0.04221651908878972</v>
       </c>
       <c r="G95" t="n">
-        <v>0.0243889566952899</v>
+        <v>-0.03798512031056907</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>2076</v>
+        <v>8006</v>
       </c>
       <c r="B96" t="n">
-        <v>0.3552233921090318</v>
+        <v>0.2890444000982779</v>
       </c>
       <c r="C96" t="n">
-        <v>0.0005976529976346648</v>
+        <v>0.0008242750324588202</v>
       </c>
       <c r="D96" t="n">
-        <v>21.10065134583059</v>
+        <v>-20.90560573335789</v>
       </c>
       <c r="E96" t="n">
-        <v>1.061172766109138e-98</v>
+        <v>5.063863046732843e-97</v>
       </c>
       <c r="F96" t="n">
-        <v>0.01143948055854783</v>
+        <v>-0.01884752073477335</v>
       </c>
       <c r="G96" t="n">
-        <v>0.01378225449921132</v>
+        <v>-0.0156164169540964</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>2079</v>
+        <v>8066</v>
       </c>
       <c r="B97" t="n">
-        <v>0.3506818219511778</v>
+        <v>0.2892494326555759</v>
       </c>
       <c r="C97" t="n">
-        <v>0.0005780938234871564</v>
+        <v>0.000646131139163274</v>
       </c>
       <c r="D97" t="n">
-        <v>13.95845629754398</v>
+        <v>-26.35213698133549</v>
       </c>
       <c r="E97" t="n">
-        <v>2.961783248974838e-44</v>
+        <v>5.666072551730054e-153</v>
       </c>
       <c r="F97" t="n">
-        <v>0.006936245959684612</v>
+        <v>-0.01829333201935746</v>
       </c>
       <c r="G97" t="n">
-        <v>0.009202348782366537</v>
+        <v>-0.01576054055491642</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>2080</v>
+        <v>8102</v>
       </c>
       <c r="B98" t="n">
-        <v>0.2989346893023642</v>
+        <v>0.3368142866113399</v>
       </c>
       <c r="C98" t="n">
-        <v>0.0006888293686149376</v>
+        <v>0.000635744897491971</v>
       </c>
       <c r="D98" t="n">
-        <v>-63.40878781869179</v>
+        <v>48.03486082090462</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>-0.04502792596648329</v>
+        <v>0.02929187862768659</v>
       </c>
       <c r="G98" t="n">
-        <v>-0.04232774458909274</v>
+        <v>0.03178395670956761</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>2094</v>
+        <v>8226</v>
       </c>
       <c r="B99" t="n">
-        <v>0.3384913437900307</v>
+        <v>0.3439205729327833</v>
       </c>
       <c r="C99" t="n">
-        <v>0.0005413902974399332</v>
+        <v>0.0007145322967704212</v>
       </c>
       <c r="D99" t="n">
-        <v>-7.612217672923419</v>
+        <v>52.68369835795622</v>
       </c>
       <c r="E99" t="n">
-        <v>2.708578351953788e-14</v>
+        <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>-0.005182294082943704</v>
+        <v>0.03624374424387165</v>
       </c>
       <c r="G99" t="n">
-        <v>-0.003060067497299347</v>
+        <v>0.0390446637362694</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>2103</v>
+        <v>4143</v>
       </c>
       <c r="B100" t="n">
-        <v>0.3392387374976286</v>
-      </c>
-      <c r="C100" t="n">
-        <v>0.0005235756015487769</v>
-      </c>
-      <c r="D100" t="n">
-        <v>-6.443743888263117</v>
-      </c>
-      <c r="E100" t="n">
-        <v>1.16882108339801e-10</v>
-      </c>
-      <c r="F100" t="n">
-        <v>-0.004399983956069204</v>
-      </c>
-      <c r="G100" t="n">
-        <v>-0.002347590208978028</v>
-      </c>
+        <v>0.3062763689427128</v>
+      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1381</v>
+        <v>26</v>
       </c>
       <c r="B101" t="n">
-        <v>0.3426125245801522</v>
-      </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr"/>
+        <v>0.3526890958874039</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.0009041199987723246</v>
+      </c>
+      <c r="D101" t="n">
+        <v>114.4673977975002</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.1017202151056228</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0.1052643120066714</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>997</v>
+        <v>47</v>
       </c>
       <c r="B102" t="n">
-        <v>0.3066511400184093</v>
+        <v>0.3630501035502399</v>
       </c>
       <c r="C102" t="n">
-        <v>0.0007770198896791958</v>
+        <v>0.0009044580184232652</v>
       </c>
       <c r="D102" t="n">
-        <v>-37.18646509716957</v>
+        <v>125.8801059859723</v>
       </c>
       <c r="E102" t="n">
-        <v>2.599266380259235e-301</v>
+        <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>-0.03041756615482561</v>
+        <v>0.1120805602599428</v>
       </c>
       <c r="G102" t="n">
-        <v>-0.02737167985989833</v>
+        <v>0.1156259821780234</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1001</v>
+        <v>641</v>
       </c>
       <c r="B103" t="n">
-        <v>0.338229203356046</v>
+        <v>0.3329365433005321</v>
       </c>
       <c r="C103" t="n">
-        <v>0.0007258127296560317</v>
+        <v>0.0008975507085357812</v>
       </c>
       <c r="D103" t="n">
-        <v>3.697152475606849</v>
+        <v>93.29802781380901</v>
       </c>
       <c r="E103" t="n">
-        <v>0.0002181081232340494</v>
+        <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>0.001260862172812276</v>
+        <v>0.08198053813327176</v>
       </c>
       <c r="G103" t="n">
-        <v>0.004106018487737248</v>
+        <v>0.08549888380527883</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>1008</v>
+        <v>642</v>
       </c>
       <c r="B104" t="n">
-        <v>0.2803698187861226</v>
+        <v>0.2663956619744592</v>
       </c>
       <c r="C104" t="n">
-        <v>0.0007371260316117494</v>
+        <v>0.001051018635684171</v>
       </c>
       <c r="D104" t="n">
-        <v>-74.85279568679003</v>
+        <v>16.36396259711102</v>
       </c>
       <c r="E104" t="n">
-        <v>0</v>
+        <v>3.632201545286527e-60</v>
       </c>
       <c r="F104" t="n">
-        <v>-0.05662069623836986</v>
+        <v>0.0151388642101125</v>
       </c>
       <c r="G104" t="n">
-        <v>-0.05373119224092737</v>
+        <v>0.01925879507629236</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>1010</v>
+        <v>645</v>
       </c>
       <c r="B105" t="n">
-        <v>0.3229252936400987</v>
+        <v>0.3359575623720246</v>
       </c>
       <c r="C105" t="n">
-        <v>0.0007405036150416793</v>
+        <v>0.0009134566466352226</v>
       </c>
       <c r="D105" t="n">
-        <v>-17.04308949924866</v>
+        <v>94.98067627003057</v>
       </c>
       <c r="E105" t="n">
-        <v>4.524111690476109e-65</v>
+        <v>0</v>
       </c>
       <c r="F105" t="n">
-        <v>-0.01407184137907849</v>
+        <v>0.0849703820366433</v>
       </c>
       <c r="G105" t="n">
-        <v>-0.01116909739226655</v>
+        <v>0.08855107804489228</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1012</v>
+        <v>699</v>
       </c>
       <c r="B106" t="n">
-        <v>0.2971049704663969</v>
+        <v>0.2785963991250318</v>
       </c>
       <c r="C106" t="n">
-        <v>0.0007156319511581006</v>
+        <v>0.001147086670056706</v>
       </c>
       <c r="D106" t="n">
-        <v>-53.7158695851491</v>
+        <v>25.62976936374093</v>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
+        <v>9.52821863538231e-145</v>
       </c>
       <c r="F106" t="n">
-        <v>-0.03984341659847355</v>
+        <v>0.02715131085534733</v>
       </c>
       <c r="G106" t="n">
-        <v>-0.0370381685202751</v>
+        <v>0.03164782273220259</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1043</v>
+        <v>703</v>
       </c>
       <c r="B107" t="n">
-        <v>0.3382744179738829</v>
+        <v>0.3725256581716542</v>
       </c>
       <c r="C107" t="n">
-        <v>0.0007518542675332874</v>
+        <v>0.0009154073235912451</v>
       </c>
       <c r="D107" t="n">
-        <v>3.629233836849684</v>
+        <v>134.7256272285049</v>
       </c>
       <c r="E107" t="n">
-        <v>0.0002843569729117027</v>
+        <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>0.001255035907157801</v>
+        <v>0.1215346545671471</v>
       </c>
       <c r="G107" t="n">
-        <v>0.004202273989065483</v>
+        <v>0.1251229971136478</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>1048</v>
+        <v>708</v>
       </c>
       <c r="B108" t="n">
-        <v>0.321439516548937</v>
+        <v>0.3464138325927043</v>
       </c>
       <c r="C108" t="n">
-        <v>0.0007393974663984676</v>
+        <v>0.0009073740830278849</v>
       </c>
       <c r="D108" t="n">
-        <v>-19.07802923040076</v>
+        <v>107.14103706493</v>
       </c>
       <c r="E108" t="n">
-        <v>4.786757188587522e-81</v>
+        <v>0</v>
       </c>
       <c r="F108" t="n">
-        <v>-0.01555545044144373</v>
+        <v>0.09543857390204963</v>
       </c>
       <c r="G108" t="n">
-        <v>-0.01265704251222473</v>
+        <v>0.09899542662084537</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1073</v>
+        <v>709</v>
       </c>
       <c r="B109" t="n">
-        <v>0.06410199720976939</v>
+        <v>0.3698177876620753</v>
       </c>
       <c r="C109" t="n">
-        <v>0.0008747970211544655</v>
+        <v>0.0008975079892930481</v>
       </c>
       <c r="D109" t="n">
-        <v>-310.2934272201553</v>
+        <v>134.3954112607171</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
       </c>
       <c r="F109" t="n">
-        <v>-0.2731583501483782</v>
+        <v>0.1188618662232669</v>
       </c>
       <c r="G109" t="n">
-        <v>-0.2697291814836254</v>
+        <v>0.12238004443837</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>1081</v>
+        <v>710</v>
       </c>
       <c r="B110" t="n">
-        <v>0.3527895970958955</v>
+        <v>0.381220875103461</v>
       </c>
       <c r="C110" t="n">
-        <v>0.0007970516733551503</v>
+        <v>0.0009079776610783541</v>
       </c>
       <c r="D110" t="n">
-        <v>21.63452464447778</v>
+        <v>145.404505453809</v>
       </c>
       <c r="E110" t="n">
-        <v>1.220766629868056e-103</v>
+        <v>0</v>
       </c>
       <c r="F110" t="n">
-        <v>0.01568162903492005</v>
+        <v>0.1302444334176834</v>
       </c>
       <c r="G110" t="n">
-        <v>0.01880603910532846</v>
+        <v>0.1338036521267251</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>1091</v>
+        <v>727</v>
       </c>
       <c r="B111" t="n">
-        <v>0.4056615705118913</v>
+        <v>0.3525530312111905</v>
       </c>
       <c r="C111" t="n">
-        <v>0.0008626162067168127</v>
+        <v>0.001053208390554255</v>
       </c>
       <c r="D111" t="n">
-        <v>81.28273841849851</v>
+        <v>98.13461401075817</v>
       </c>
       <c r="E111" t="n">
         <v>0</v>
       </c>
       <c r="F111" t="n">
-        <v>0.06842509730178643</v>
+        <v>0.1012919415920791</v>
       </c>
       <c r="G111" t="n">
-        <v>0.0718065176704538</v>
+        <v>0.1054204561677883</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>1104</v>
+        <v>728</v>
       </c>
       <c r="B112" t="n">
-        <v>0.3112964354636555</v>
+        <v>0.3556064557840622</v>
       </c>
       <c r="C112" t="n">
-        <v>0.0007748712544685477</v>
+        <v>0.0009138055068300026</v>
       </c>
       <c r="D112" t="n">
-        <v>-31.29465368895029</v>
+        <v>116.4466865842614</v>
       </c>
       <c r="E112" t="n">
-        <v>2.669869843645036e-214</v>
+        <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>-0.02576805942835741</v>
+        <v>0.1046185916930197</v>
       </c>
       <c r="G112" t="n">
-        <v>-0.02273059569587394</v>
+        <v>0.1082006552125911</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>1241</v>
+        <v>733</v>
       </c>
       <c r="B113" t="n">
-        <v>0.3407330012147606</v>
+        <v>0.3365890341092193</v>
       </c>
       <c r="C113" t="n">
-        <v>0.0008130035042503227</v>
+        <v>0.001008454242587363</v>
       </c>
       <c r="D113" t="n">
-        <v>6.380339275133401</v>
+        <v>86.65956082820652</v>
       </c>
       <c r="E113" t="n">
-        <v>1.772026409628774e-10</v>
+        <v>0</v>
       </c>
       <c r="F113" t="n">
-        <v>0.003593767890342174</v>
+        <v>0.0854156612961369</v>
       </c>
       <c r="G113" t="n">
-        <v>0.006780708487636662</v>
+        <v>0.08936874225978805</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>1295</v>
+        <v>861</v>
       </c>
       <c r="B114" t="n">
-        <v>0.3122816193197741</v>
+        <v>0.3219298738451588</v>
       </c>
       <c r="C114" t="n">
-        <v>0.001194522717467818</v>
+        <v>0.0009062450338773089</v>
       </c>
       <c r="D114" t="n">
-        <v>-19.47568126231462</v>
+        <v>80.25758905703296</v>
       </c>
       <c r="E114" t="n">
-        <v>2.23980233270879e-84</v>
+        <v>0</v>
       </c>
       <c r="F114" t="n">
-        <v>-0.02560538388687374</v>
+        <v>0.07095682805743797</v>
       </c>
       <c r="G114" t="n">
-        <v>-0.02092290352512048</v>
+        <v>0.07450925497036598</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>1355</v>
+        <v>862</v>
       </c>
       <c r="B115" t="n">
-        <v>0.3340193985104942</v>
+        <v>0.3780464767044284</v>
       </c>
       <c r="C115" t="n">
-        <v>0.0007366294096437343</v>
+        <v>0.0009708426443954089</v>
       </c>
       <c r="D115" t="n">
-        <v>-2.072092826181432</v>
+        <v>132.7193908477439</v>
       </c>
       <c r="E115" t="n">
-        <v>0.03825847031571212</v>
+        <v>0</v>
       </c>
       <c r="F115" t="n">
-        <v>-0.00297014314506255</v>
+        <v>0.126946821511118</v>
       </c>
       <c r="G115" t="n">
-        <v>-8.258588549154102e-05</v>
+        <v>0.1307524672352251</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>1356</v>
+        <v>863</v>
       </c>
       <c r="B116" t="n">
-        <v>0.3375626258918082</v>
+        <v>0.3340264486744362</v>
       </c>
       <c r="C116" t="n">
-        <v>0.0007510595520850479</v>
+        <v>0.0009249135229754341</v>
       </c>
       <c r="D116" t="n">
-        <v>2.685356787538185</v>
+        <v>91.71626777634698</v>
       </c>
       <c r="E116" t="n">
-        <v>0.007246029391261294</v>
+        <v>0</v>
       </c>
       <c r="F116" t="n">
-        <v>0.0005448014511647233</v>
+        <v>0.08301681320036301</v>
       </c>
       <c r="G116" t="n">
-        <v>0.003488924280909222</v>
+        <v>0.08664241948599573</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>1357</v>
+        <v>864</v>
       </c>
       <c r="B117" t="n">
-        <v>0.3115241678690934</v>
+        <v>0.269824277664631</v>
       </c>
       <c r="C117" t="n">
-        <v>0.0009681263866999754</v>
+        <v>0.00090861472735207</v>
       </c>
       <c r="D117" t="n">
-        <v>-24.81245784298836</v>
+        <v>22.70208121487061</v>
       </c>
       <c r="E117" t="n">
-        <v>1.228813332673313e-135</v>
+        <v>5.118438846202889e-114</v>
       </c>
       <c r="F117" t="n">
-        <v>-0.02591910314339379</v>
+        <v>0.01884658734780359</v>
       </c>
       <c r="G117" t="n">
-        <v>-0.02212408716996178</v>
+        <v>0.02240830331894483</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>1374</v>
+        <v>874</v>
       </c>
       <c r="B118" t="n">
-        <v>0.3148902966474396</v>
+        <v>0.3298879209862977</v>
       </c>
       <c r="C118" t="n">
-        <v>0.0009301972159905117</v>
+        <v>0.001097038762736038</v>
       </c>
       <c r="D118" t="n">
-        <v>-22.20547000491377</v>
+        <v>73.55354377250593</v>
       </c>
       <c r="E118" t="n">
-        <v>4.54270558182306e-109</v>
+        <v>0</v>
       </c>
       <c r="F118" t="n">
-        <v>-0.0224786339634849</v>
+        <v>0.07854092513436758</v>
       </c>
       <c r="G118" t="n">
-        <v>-0.01883229879317829</v>
+        <v>0.08284125217571428</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>1378</v>
+        <v>876</v>
       </c>
       <c r="B119" t="n">
-        <v>0.3471386682558686</v>
+        <v>0.328942226422102</v>
       </c>
       <c r="C119" t="n">
-        <v>0.0008227704900534983</v>
+        <v>0.0009199880393676573</v>
       </c>
       <c r="D119" t="n">
-        <v>14.09008389367931</v>
+        <v>86.68090309701982</v>
       </c>
       <c r="E119" t="n">
-        <v>4.666434498617692e-45</v>
+        <v>0</v>
       </c>
       <c r="F119" t="n">
-        <v>0.009980291838335202</v>
+        <v>0.07794224475018681</v>
       </c>
       <c r="G119" t="n">
-        <v>0.01320551862185965</v>
+        <v>0.08154854343150351</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>1379</v>
+        <v>887</v>
       </c>
       <c r="B120" t="n">
-        <v>0.2764575811362163</v>
+        <v>0.3237914567309769</v>
       </c>
       <c r="C120" t="n">
-        <v>0.0007566612753488547</v>
+        <v>0.0009478289261570252</v>
       </c>
       <c r="D120" t="n">
-        <v>-78.09066462706534</v>
+        <v>78.70051476711539</v>
       </c>
       <c r="E120" t="n">
         <v>0</v>
       </c>
       <c r="F120" t="n">
-        <v>-0.06057122256785651</v>
+        <v>0.07273690774458655</v>
       </c>
       <c r="G120" t="n">
-        <v>-0.05760514121125339</v>
+        <v>0.07645234105485363</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>995</v>
+        <v>889</v>
       </c>
       <c r="B121" t="n">
-        <v>0.3355457630257712</v>
-      </c>
-      <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr"/>
-      <c r="E121" t="inlineStr"/>
-      <c r="F121" t="inlineStr"/>
-      <c r="G121" t="inlineStr"/>
+        <v>0.3692496139220787</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0.0009101140573705894</v>
+      </c>
+      <c r="D121" t="n">
+        <v>131.9096003611529</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0.1182689849627704</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0.1218365782188733</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>710</v>
+        <v>892</v>
       </c>
       <c r="B122" t="n">
-        <v>0.3922628957803921</v>
+        <v>0.3339074831160977</v>
       </c>
       <c r="C122" t="n">
-        <v>0.0008055272057873696</v>
+        <v>0.0009127106273386031</v>
       </c>
       <c r="D122" t="n">
-        <v>13.00232827138484</v>
+        <v>92.81216658104543</v>
       </c>
       <c r="E122" t="n">
-        <v>1.247185955844668e-38</v>
+        <v>0</v>
       </c>
       <c r="F122" t="n">
-        <v>0.008894911708673988</v>
+        <v>0.08292176495646791</v>
       </c>
       <c r="G122" t="n">
-        <v>0.01205254661368352</v>
+        <v>0.08649953661321391</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>727</v>
+        <v>897</v>
       </c>
       <c r="B123" t="n">
-        <v>0.3684147463455847</v>
+        <v>0.3059805376890877</v>
       </c>
       <c r="C123" t="n">
-        <v>0.001014509790916931</v>
+        <v>0.00163479162337327</v>
       </c>
       <c r="D123" t="n">
-        <v>-13.18313573054876</v>
+        <v>34.73452184729328</v>
       </c>
       <c r="E123" t="n">
-        <v>1.156457519069081e-39</v>
+        <v>6.364510668929966e-264</v>
       </c>
       <c r="F123" t="n">
-        <v>-0.01536283947552376</v>
+        <v>0.05357956213894142</v>
       </c>
       <c r="G123" t="n">
-        <v>-0.01138600107173332</v>
+        <v>0.05998784857672037</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>728</v>
+        <v>983</v>
       </c>
       <c r="B124" t="n">
-        <v>0.3708559985405951</v>
+        <v>0.3589171486030052</v>
       </c>
       <c r="C124" t="n">
-        <v>0.0008173529031306992</v>
+        <v>0.0009632847875867139</v>
       </c>
       <c r="D124" t="n">
-        <v>-13.37631277351681</v>
+        <v>113.9022620160203</v>
       </c>
       <c r="E124" t="n">
-        <v>8.792791245627881e-41</v>
+        <v>0</v>
       </c>
       <c r="F124" t="n">
-        <v>-0.012535163664921</v>
+        <v>0.1078323065854517</v>
       </c>
       <c r="G124" t="n">
-        <v>-0.009331172492315428</v>
+        <v>0.111608325958045</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>733</v>
+        <v>988</v>
       </c>
       <c r="B125" t="n">
-        <v>0.3515552453893928</v>
+        <v>0.3746252827709241</v>
       </c>
       <c r="C125" t="n">
-        <v>0.0009467932390692772</v>
+        <v>0.0009169960356342063</v>
       </c>
       <c r="D125" t="n">
-        <v>-31.93297119394435</v>
+        <v>136.7818895235675</v>
       </c>
       <c r="E125" t="n">
-        <v>5.537242491497931e-223</v>
+        <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>-0.03208961732427452</v>
+        <v>0.1236311653378125</v>
       </c>
       <c r="G125" t="n">
-        <v>-0.02837822513536646</v>
+        <v>0.1272257355415222</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>861</v>
+        <v>990</v>
       </c>
       <c r="B126" t="n">
-        <v>0.3329206528608299</v>
+        <v>0.3368810586730958</v>
       </c>
       <c r="C126" t="n">
-        <v>0.0007957256963035465</v>
+        <v>0.0008979216752439488</v>
       </c>
       <c r="D126" t="n">
-        <v>-61.41376857049679</v>
+        <v>97.65242198660238</v>
       </c>
       <c r="E126" t="n">
         <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>-0.05042812044541338</v>
+        <v>0.08592432642206201</v>
       </c>
       <c r="G126" t="n">
-        <v>-0.04730890707135345</v>
+        <v>0.08944412626161606</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>862</v>
+        <v>991</v>
       </c>
       <c r="B127" t="n">
-        <v>0.3907917437844748</v>
+        <v>0.3908690037108465</v>
       </c>
       <c r="C127" t="n">
-        <v>0.0008947408106495886</v>
+        <v>0.0009307472794970796</v>
       </c>
       <c r="D127" t="n">
-        <v>10.06165926278197</v>
+        <v>152.2133607053259</v>
       </c>
       <c r="E127" t="n">
-        <v>8.308986058418837e-24</v>
+        <v>0</v>
       </c>
       <c r="F127" t="n">
-        <v>0.007248902804951031</v>
+        <v>0.1398479342465741</v>
       </c>
       <c r="G127" t="n">
-        <v>0.01075625152557193</v>
+        <v>0.1434964085126053</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>863</v>
+        <v>994</v>
       </c>
       <c r="B128" t="n">
-        <v>0.3444373786248239</v>
+        <v>0.3334619279238277</v>
       </c>
       <c r="C128" t="n">
-        <v>0.000836512996245232</v>
+        <v>0.0009011246565874869</v>
       </c>
       <c r="D128" t="n">
-        <v>-44.65177249133782</v>
+        <v>93.51103088409378</v>
       </c>
       <c r="E128" t="n">
         <v>0</v>
       </c>
       <c r="F128" t="n">
-        <v>-0.03899133698569642</v>
+        <v>0.08249891792411605</v>
       </c>
       <c r="G128" t="n">
-        <v>-0.03571223900308244</v>
+        <v>0.08603127326102573</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>864</v>
+        <v>995</v>
       </c>
       <c r="B129" t="n">
-        <v>0.2856383234560545</v>
+        <v>0.3432046785664058</v>
       </c>
       <c r="C129" t="n">
-        <v>0.0008206002111289254</v>
+        <v>0.0009022662626515629</v>
       </c>
       <c r="D129" t="n">
-        <v>-117.1713604982883</v>
+        <v>104.1908027890575</v>
       </c>
       <c r="E129" t="n">
         <v>0</v>
       </c>
       <c r="F129" t="n">
-        <v>-0.09775920340915828</v>
+        <v>0.09223943105258128</v>
       </c>
       <c r="G129" t="n">
-        <v>-0.09454248291715933</v>
+        <v>0.09577626141771664</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>874</v>
+        <v>997</v>
       </c>
       <c r="B130" t="n">
-        <v>0.3450804746357217</v>
+        <v>0.317999539281411</v>
       </c>
       <c r="C130" t="n">
-        <v>0.00106417367204245</v>
+        <v>0.0009275343746279347</v>
       </c>
       <c r="D130" t="n">
-        <v>-34.49501988997463</v>
+        <v>74.17806696140319</v>
       </c>
       <c r="E130" t="n">
-        <v>1.076632971405328e-259</v>
+        <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>-0.03879445141389404</v>
+        <v>0.06698476701563298</v>
       </c>
       <c r="G130" t="n">
-        <v>-0.03462293255308924</v>
+        <v>0.07062064688467536</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>876</v>
+        <v>1001</v>
       </c>
       <c r="B131" t="n">
-        <v>0.3442111472284512</v>
+        <v>0.3473497030752567</v>
       </c>
       <c r="C131" t="n">
-        <v>0.0008232067301321363</v>
+        <v>0.0009006506067338913</v>
       </c>
       <c r="D131" t="n">
-        <v>-45.64833840064731</v>
+        <v>108.9799640505882</v>
       </c>
       <c r="E131" t="n">
         <v>0</v>
       </c>
       <c r="F131" t="n">
-        <v>-0.03919148836265313</v>
+        <v>0.09638762219923405</v>
       </c>
       <c r="G131" t="n">
-        <v>-0.03596455041887108</v>
+        <v>0.09991811928876579</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>887</v>
+        <v>1008</v>
       </c>
       <c r="B132" t="n">
-        <v>0.3241253316874334</v>
+        <v>0.2868890623473828</v>
       </c>
       <c r="C132" t="n">
-        <v>0.0009175331906211271</v>
+        <v>0.0009126588832240599</v>
       </c>
       <c r="D132" t="n">
-        <v>-62.84659293114419</v>
+        <v>41.29936245508767</v>
       </c>
       <c r="E132" t="n">
         <v>0</v>
       </c>
       <c r="F132" t="n">
-        <v>-0.05946218190776943</v>
+        <v>0.03590344560468671</v>
       </c>
       <c r="G132" t="n">
-        <v>-0.05586548795579037</v>
+        <v>0.03948101442756526</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>889</v>
+        <v>1010</v>
       </c>
       <c r="B133" t="n">
-        <v>0.376287439160477</v>
+        <v>0.3363420562228316</v>
       </c>
       <c r="C133" t="n">
-        <v>0.0008053893598754037</v>
+        <v>0.0008999537920368665</v>
       </c>
       <c r="D133" t="n">
-        <v>-6.831139983755774</v>
+        <v>96.83299816353784</v>
       </c>
       <c r="E133" t="n">
-        <v>8.4571806376492e-12</v>
+        <v>0</v>
       </c>
       <c r="F133" t="n">
-        <v>-0.007080274735969548</v>
+        <v>0.08538134108300087</v>
       </c>
       <c r="G133" t="n">
-        <v>-0.003923180181503129</v>
+        <v>0.08890910670014875</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>892</v>
+        <v>1012</v>
       </c>
       <c r="B134" t="n">
-        <v>0.3435192143440927</v>
+        <v>0.3019609409403698</v>
       </c>
       <c r="C134" t="n">
-        <v>0.0008743014899139044</v>
+        <v>0.0009072036910842289</v>
       </c>
       <c r="D134" t="n">
-        <v>-43.77203140633921</v>
+        <v>58.16125874229292</v>
       </c>
       <c r="E134" t="n">
         <v>0</v>
       </c>
       <c r="F134" t="n">
-        <v>-0.03998356596949326</v>
+        <v>0.05098601621288391</v>
       </c>
       <c r="G134" t="n">
-        <v>-0.03655633858074792</v>
+        <v>0.05454220100534211</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>897</v>
+        <v>1043</v>
       </c>
       <c r="B135" t="n">
-        <v>0.3289886920030129</v>
+        <v>0.3454000754683467</v>
       </c>
       <c r="C135" t="n">
-        <v>0.001978914857231903</v>
+        <v>0.0009148833909391086</v>
       </c>
       <c r="D135" t="n">
-        <v>-26.68152923469253</v>
+        <v>105.1535573712179</v>
       </c>
       <c r="E135" t="n">
-        <v>1.842238979585716e-156</v>
+        <v>0</v>
       </c>
       <c r="F135" t="n">
-        <v>-0.05667910874695554</v>
+        <v>0.09441009875633796</v>
       </c>
       <c r="G135" t="n">
-        <v>-0.04892184048544528</v>
+        <v>0.09799638751784187</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>983</v>
+        <v>1048</v>
       </c>
       <c r="B136" t="n">
-        <v>0.3588998738965387</v>
+        <v>0.3288314420744395</v>
       </c>
       <c r="C136" t="n">
-        <v>0.0009477570438127105</v>
+        <v>0.0009214833366143637</v>
       </c>
       <c r="D136" t="n">
-        <v>-24.15101303873599</v>
+        <v>86.4200214794653</v>
       </c>
       <c r="E136" t="n">
-        <v>1.308193736862381e-128</v>
+        <v>0</v>
       </c>
       <c r="F136" t="n">
-        <v>-0.02474687785543652</v>
+        <v>0.07782852966415697</v>
       </c>
       <c r="G136" t="n">
-        <v>-0.02103170758991278</v>
+        <v>0.08144068982220838</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>988</v>
+        <v>1073</v>
       </c>
       <c r="B137" t="n">
-        <v>0.3896098951548316</v>
+        <v>0.07900444149154218</v>
       </c>
       <c r="C137" t="n">
-        <v>0.0008880228516007071</v>
+        <v>0.0009555594198968467</v>
       </c>
       <c r="D137" t="n">
-        <v>8.806900094430006</v>
+        <v>-178.1075957140237</v>
       </c>
       <c r="E137" t="n">
-        <v>1.300256743826932e-18</v>
+        <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>0.006080221242683551</v>
+        <v>-0.1720652590338829</v>
       </c>
       <c r="G137" t="n">
-        <v>0.009561235828552991</v>
+        <v>-0.1683195226455464</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>990</v>
+        <v>1081</v>
       </c>
       <c r="B138" t="n">
-        <v>0.3590823302196161</v>
+        <v>0.3677167609983559</v>
       </c>
       <c r="C138" t="n">
-        <v>0.0009726525605035621</v>
+        <v>0.0009287717043241525</v>
       </c>
       <c r="D138" t="n">
-        <v>-23.34526975165871</v>
+        <v>127.6093232764272</v>
       </c>
       <c r="E138" t="n">
-        <v>2.566674165194171e-120</v>
+        <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>-0.02461321625457111</v>
+        <v>0.1166995636029779</v>
       </c>
       <c r="G138" t="n">
-        <v>-0.02080045654462328</v>
+        <v>0.1203402937312203</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>991</v>
+        <v>1091</v>
       </c>
       <c r="B139" t="n">
-        <v>0.4126613373984258</v>
+        <v>0.4205640147936579</v>
       </c>
       <c r="C139" t="n">
-        <v>0.000934162087984787</v>
+        <v>0.0009442385678985268</v>
       </c>
       <c r="D139" t="n">
-        <v>33.0479808336166</v>
+        <v>181.4871667906888</v>
       </c>
       <c r="E139" t="n">
-        <v>1.284313959253424e-238</v>
+        <v>0</v>
       </c>
       <c r="F139" t="n">
-        <v>0.02904123149201978</v>
+        <v>0.1695165028032387</v>
       </c>
       <c r="G139" t="n">
-        <v>0.03270311006640523</v>
+        <v>0.1732178621215635</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>994</v>
+        <v>1104</v>
       </c>
       <c r="B140" t="n">
-        <v>0.3499014273836196</v>
+        <v>0.3235832572137894</v>
       </c>
       <c r="C140" t="n">
-        <v>0.0008263639639450703</v>
+        <v>0.0009286733738833521</v>
       </c>
       <c r="D140" t="n">
-        <v>-38.58800798060135</v>
+        <v>80.09966364328662</v>
       </c>
       <c r="E140" t="n">
         <v>0</v>
       </c>
       <c r="F140" t="n">
-        <v>-0.03350739632355295</v>
+        <v>0.0725662525431665</v>
       </c>
       <c r="G140" t="n">
-        <v>-0.03026808214763452</v>
+        <v>0.07620659722189883</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>709</v>
+        <v>1241</v>
       </c>
       <c r="B141" t="n">
-        <v>0.3817891666192133</v>
-      </c>
-      <c r="C141" t="inlineStr"/>
-      <c r="D141" t="inlineStr"/>
-      <c r="E141" t="inlineStr"/>
-      <c r="F141" t="inlineStr"/>
-      <c r="G141" t="inlineStr"/>
+        <v>0.3560232415045217</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.0009470716479367335</v>
+      </c>
+      <c r="D141" t="n">
+        <v>112.7965443860495</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0.1049701767610401</v>
+      </c>
+      <c r="G141" t="n">
+        <v>0.1086826415854896</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>26</v>
+        <v>1295</v>
       </c>
       <c r="B142" t="n">
-        <v>0.349760668380967</v>
+        <v>0.3269675600284173</v>
       </c>
       <c r="C142" t="n">
-        <v>0.0007709865219043942</v>
+        <v>0.001269422569784558</v>
       </c>
       <c r="D142" t="n">
-        <v>123.4993857154247</v>
+        <v>61.26464862709941</v>
       </c>
       <c r="E142" t="n">
         <v>0</v>
       </c>
       <c r="F142" t="n">
-        <v>0.09370522990906471</v>
+        <v>0.0752826970143952</v>
       </c>
       <c r="G142" t="n">
-        <v>0.09672749379106438</v>
+        <v>0.08025875837992587</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>47</v>
+        <v>1355</v>
       </c>
       <c r="B143" t="n">
-        <v>0.3596437002210764</v>
+        <v>0.3472713044811945</v>
       </c>
       <c r="C143" t="n">
-        <v>0.0007689872623041464</v>
+        <v>0.0008962431477787718</v>
       </c>
       <c r="D143" t="n">
-        <v>136.672476700408</v>
+        <v>109.4284206166632</v>
       </c>
       <c r="E143" t="n">
         <v>0</v>
       </c>
       <c r="F143" t="n">
-        <v>0.1035921802937329</v>
+        <v>0.09631786209433557</v>
       </c>
       <c r="G143" t="n">
-        <v>0.106606607086615</v>
+        <v>0.09983108220553971</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>641</v>
+        <v>1356</v>
       </c>
       <c r="B144" t="n">
-        <v>0.3301854777743005</v>
+        <v>0.3515986155479254</v>
       </c>
       <c r="C144" t="n">
-        <v>0.0007473525491001789</v>
+        <v>0.0009041240525544935</v>
       </c>
       <c r="D144" t="n">
-        <v>101.2121673157746</v>
+        <v>113.2607665146665</v>
       </c>
       <c r="E144" t="n">
         <v>0</v>
       </c>
       <c r="F144" t="n">
-        <v>0.07417636183876228</v>
+        <v>0.1006297268208511</v>
       </c>
       <c r="G144" t="n">
-        <v>0.07710598064803367</v>
+        <v>0.104173839612486</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>642</v>
+        <v>1357</v>
       </c>
       <c r="B145" t="n">
-        <v>0.2636385847908201</v>
+        <v>0.3266157822446445</v>
       </c>
       <c r="C145" t="n">
-        <v>0.001280055664691133</v>
+        <v>0.001052507854671631</v>
       </c>
       <c r="D145" t="n">
-        <v>7.104595925609242</v>
+        <v>73.55664812358235</v>
       </c>
       <c r="E145" t="n">
-        <v>1.218209705798552e-12</v>
+        <v>0</v>
       </c>
       <c r="F145" t="n">
-        <v>0.006585371883195801</v>
+        <v>0.07535606565513876</v>
       </c>
       <c r="G145" t="n">
-        <v>0.01160318463663951</v>
+        <v>0.07948183417163672</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>645</v>
+        <v>1374</v>
       </c>
       <c r="B146" t="n">
-        <v>0.3318314188374855</v>
+        <v>0.3194418030454734</v>
       </c>
       <c r="C146" t="n">
-        <v>0.0008031231838175372</v>
+        <v>0.001015418857446731</v>
       </c>
       <c r="D146" t="n">
-        <v>96.23319792514171</v>
+        <v>69.17832005882518</v>
       </c>
       <c r="E146" t="n">
         <v>0</v>
       </c>
       <c r="F146" t="n">
-        <v>0.07571299257667334</v>
+        <v>0.06825477979330458</v>
       </c>
       <c r="G146" t="n">
-        <v>0.07886123203649271</v>
+        <v>0.07223516163512855</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>699</v>
+        <v>1378</v>
       </c>
       <c r="B147" t="n">
-        <v>0.2750704595965284</v>
+        <v>0.3628857773739312</v>
       </c>
       <c r="C147" t="n">
-        <v>0.00111318631671998</v>
+        <v>0.0009713811459892785</v>
       </c>
       <c r="D147" t="n">
-        <v>18.43909932894844</v>
+        <v>117.0384513968415</v>
       </c>
       <c r="E147" t="n">
-        <v>9.65023888240185e-76</v>
+        <v>0</v>
       </c>
       <c r="F147" t="n">
-        <v>0.01834431025555398</v>
+        <v>0.1117850667334277</v>
       </c>
       <c r="G147" t="n">
-        <v>0.02270799587569796</v>
+        <v>0.1155928233519211</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>703</v>
+        <v>1379</v>
       </c>
       <c r="B148" t="n">
-        <v>0.3685340634276624</v>
+        <v>0.291291533239852</v>
       </c>
       <c r="C148" t="n">
-        <v>0.0008032989302633499</v>
+        <v>0.0009021302645789553</v>
       </c>
       <c r="D148" t="n">
-        <v>141.9020399534081</v>
+        <v>46.66144409670338</v>
       </c>
       <c r="E148" t="n">
         <v>0</v>
       </c>
       <c r="F148" t="n">
-        <v>0.1124152927041907</v>
+        <v>0.04032655227822649</v>
       </c>
       <c r="G148" t="n">
-        <v>0.1155642210893291</v>
+        <v>0.04386284953896383</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>708</v>
+        <v>1381</v>
       </c>
       <c r="B149" t="n">
-        <v>0.3423899489187325</v>
+        <v>0.3462595841395122</v>
       </c>
       <c r="C149" t="n">
-        <v>0.0007604340613835718</v>
+        <v>0.000963952107060587</v>
       </c>
       <c r="D149" t="n">
-        <v>115.5203940076005</v>
+        <v>100.6925044276653</v>
       </c>
       <c r="E149" t="n">
         <v>0</v>
       </c>
       <c r="F149" t="n">
-        <v>0.08635519324697796</v>
+        <v>0.09517343419553165</v>
       </c>
       <c r="G149" t="n">
-        <v>0.08933609152868213</v>
+        <v>0.09895206942097917</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>4143</v>
+        <v>7</v>
       </c>
       <c r="B150" t="n">
-        <v>0.2919304536840664</v>
-      </c>
-      <c r="C150" t="n">
-        <v>0.0007192830020503469</v>
-      </c>
-      <c r="D150" t="n">
-        <v>51.97696462531869</v>
-      </c>
-      <c r="E150" t="n">
-        <v>0</v>
-      </c>
-      <c r="F150" t="n">
-        <v>0.03597635400096752</v>
-      </c>
-      <c r="G150" t="n">
-        <v>0.03879594030536029</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>7</v>
-      </c>
-      <c r="B151" t="n">
-        <v>0.2545443065309025</v>
-      </c>
-      <c r="C151" t="inlineStr"/>
-      <c r="D151" t="inlineStr"/>
-      <c r="E151" t="inlineStr"/>
-      <c r="F151" t="inlineStr"/>
-      <c r="G151" t="inlineStr"/>
+        <v>0.2491968323312568</v>
+      </c>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="inlineStr"/>
+      <c r="G150" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
hourly data and its code with more adjustments
</commit_message>
<xml_diff>
--- a/hourly datasets/PlantID_year-4final.xlsx
+++ b/hourly datasets/PlantID_year-4final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B147"/>
+  <dimension ref="A1:C145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,13 +444,21 @@
           <t>Coef.</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>intercept</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>8226</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3538135042719735</v>
+        <v>0.3538135330166676</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1546329437273875</v>
       </c>
     </row>
     <row r="3">
@@ -460,6 +468,9 @@
       <c r="B3" t="n">
         <v>0.3418311770192904</v>
       </c>
+      <c r="C3" t="n">
+        <v>0.2093754658246962</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -468,13 +479,19 @@
       <c r="B4" t="n">
         <v>0.2831109832446886</v>
       </c>
+      <c r="C4" t="n">
+        <v>0.2596568808986405</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>8006</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2860905931815257</v>
+        <v>0.2861244128230339</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.2117030783728674</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +499,10 @@
         <v>8002</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2811480751851599</v>
+        <v>0.2811489327152589</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1373650061817846</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +510,10 @@
         <v>6705</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3027575119428183</v>
+        <v>0.3027577199662704</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.07713924339506242</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +521,10 @@
         <v>6639</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3240999825522509</v>
+        <v>0.3241001533599427</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1687395391009784</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +532,10 @@
         <v>6195</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5141986897576902</v>
+        <v>1.13589443031268</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1922063364081459</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +543,10 @@
         <v>6155</v>
       </c>
       <c r="B10" t="n">
-        <v>0.372465875936306</v>
+        <v>0.372197564978325</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.2390211436427051</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +554,10 @@
         <v>6124</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3594934474204239</v>
+        <v>0.4459275072059499</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.3260796095772839</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +565,10 @@
         <v>6113</v>
       </c>
       <c r="B12" t="n">
-        <v>0.4221229915697143</v>
+        <v>0.4221246486283537</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.2749164335955042</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +576,10 @@
         <v>6101</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2797133937826914</v>
+        <v>0.2797165207697392</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1400301505202271</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +587,10 @@
         <v>6094</v>
       </c>
       <c r="B14" t="n">
-        <v>0.3860466347609987</v>
+        <v>0.3860563094385062</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.284698748832014</v>
       </c>
     </row>
     <row r="15">
@@ -556,13 +600,19 @@
       <c r="B15" t="n">
         <v>0.3540131886687025</v>
       </c>
+      <c r="C15" t="n">
+        <v>0.3175453004912062</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>6073</v>
       </c>
       <c r="B16" t="n">
-        <v>0.3265994324404273</v>
+        <v>0.3265982377456648</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.2158015486361115</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +620,10 @@
         <v>6061</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2997526295932063</v>
+        <v>0.2997548580286813</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.2939386487086316</v>
       </c>
     </row>
     <row r="18">
@@ -580,13 +633,19 @@
       <c r="B18" t="n">
         <v>0.3826035625465314</v>
       </c>
+      <c r="C18" t="n">
+        <v>0.3574954265024484</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>6041</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3517668622592544</v>
+        <v>0.3616478261929838</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.2740011414567843</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +653,10 @@
         <v>6025</v>
       </c>
       <c r="B20" t="n">
-        <v>0.39684147531595</v>
+        <v>0.3965486879255518</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.1934815315117472</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +664,10 @@
         <v>6018</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3359242378960482</v>
+        <v>0.3359241691763017</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.2038559471964597</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +675,10 @@
         <v>6017</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3642752606879836</v>
+        <v>0.3642751313647442</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.1796301357976015</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +686,10 @@
         <v>4271</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2878533584757698</v>
+        <v>0.2878529632520799</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.1641334652606165</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +697,10 @@
         <v>4078</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2984940845039524</v>
+        <v>0.3347993193356881</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.2746844040044751</v>
       </c>
     </row>
     <row r="25">
@@ -636,13 +710,19 @@
       <c r="B25" t="n">
         <v>0.3102934197759805</v>
       </c>
+      <c r="C25" t="n">
+        <v>0.2821073164834376</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>4057</v>
       </c>
       <c r="B26" t="n">
-        <v>0.302722950244348</v>
+        <v>0.3569403101835894</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.2832344266904956</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +730,10 @@
         <v>4054</v>
       </c>
       <c r="B27" t="n">
-        <v>0.3699931492470661</v>
+        <v>0.3699932106602539</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.2259581061908454</v>
       </c>
     </row>
     <row r="28">
@@ -660,13 +743,19 @@
       <c r="B28" t="n">
         <v>0.3533299368859437</v>
       </c>
+      <c r="C28" t="n">
+        <v>0.3641465745337381</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>4041</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3590734529574027</v>
+        <v>0.3590737138840505</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.2126324603695098</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +763,10 @@
         <v>4040</v>
       </c>
       <c r="B30" t="n">
-        <v>0.2846406863235915</v>
+        <v>0.2846702677350387</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.2356623440553718</v>
       </c>
     </row>
     <row r="31">
@@ -684,13 +776,19 @@
       <c r="B31" t="n">
         <v>0.3628827346266098</v>
       </c>
+      <c r="C31" t="n">
+        <v>0.2133958277579524</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
         <v>3948</v>
       </c>
       <c r="B32" t="n">
-        <v>0.3719551676709464</v>
+        <v>0.3719535146340285</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.2492150820300328</v>
       </c>
     </row>
     <row r="33">
@@ -700,13 +798,19 @@
       <c r="B33" t="n">
         <v>0.3974771691341019</v>
       </c>
+      <c r="C33" t="n">
+        <v>0.3791859625391745</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>3946</v>
       </c>
       <c r="B34" t="n">
-        <v>0.3645637986026317</v>
+        <v>0.3655394713647989</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.1685614844142961</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +818,10 @@
         <v>3945</v>
       </c>
       <c r="B35" t="n">
-        <v>0.2981306816538398</v>
+        <v>0.2981242612393976</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.1924259713607003</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +829,10 @@
         <v>3944</v>
       </c>
       <c r="B36" t="n">
-        <v>0.3648194038149066</v>
+        <v>0.3648328457447845</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.2581656114698205</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +840,10 @@
         <v>3943</v>
       </c>
       <c r="B37" t="n">
-        <v>0.3512546273400676</v>
+        <v>0.3512559772993038</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.2095801473789035</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +851,10 @@
         <v>3942</v>
       </c>
       <c r="B38" t="n">
-        <v>0.3407169558672337</v>
+        <v>0.3407233675796342</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.2276726085644257</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +862,10 @@
         <v>3406</v>
       </c>
       <c r="B39" t="n">
-        <v>0.3589678315352208</v>
+        <v>0.390122505563438</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.3361995570496853</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +873,10 @@
         <v>3403</v>
       </c>
       <c r="B40" t="n">
-        <v>0.375080469121677</v>
+        <v>0.3750804470195317</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.3403961674696739</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +884,10 @@
         <v>3399</v>
       </c>
       <c r="B41" t="n">
-        <v>0.3027903476571091</v>
+        <v>0.3027905338467628</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.1372195411025252</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +895,10 @@
         <v>3393</v>
       </c>
       <c r="B42" t="n">
-        <v>0.4532915149182497</v>
+        <v>0.4532756263660066</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.4428329400054485</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +906,10 @@
         <v>3181</v>
       </c>
       <c r="B43" t="n">
-        <v>0.3283255136983991</v>
+        <v>0.3283487846149303</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.1800673204823876</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +917,10 @@
         <v>3179</v>
       </c>
       <c r="B44" t="n">
-        <v>0.3697378762605237</v>
+        <v>0.3697419581629559</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.2357506535012228</v>
       </c>
     </row>
     <row r="45">
@@ -794,823 +928,1110 @@
         <v>3178</v>
       </c>
       <c r="B45" t="n">
-        <v>0.3373806530858839</v>
+        <v>0.3373794246937235</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.1771704758366996</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3148</v>
+        <v>3140</v>
       </c>
       <c r="B46" t="n">
-        <v>0.3224239125247185</v>
+        <v>0.3608692261421088</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.3227148099598149</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>3140</v>
+        <v>3131</v>
       </c>
       <c r="B47" t="n">
-        <v>0.3608692261421088</v>
+        <v>0.3560229317470405</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.3031239627150191</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>3131</v>
+        <v>3118</v>
       </c>
       <c r="B48" t="n">
-        <v>0.3560176772978677</v>
+        <v>0.3644217095493537</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.3072503879074647</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>3118</v>
+        <v>3113</v>
       </c>
       <c r="B49" t="n">
-        <v>0.3644320812603741</v>
+        <v>0.3870997564043199</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.1611534039363451</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>3113</v>
+        <v>2878</v>
       </c>
       <c r="B50" t="n">
-        <v>0.3870998161029707</v>
+        <v>0.3731426453658845</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.3766221542515145</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="B51" t="n">
-        <v>0.3731426453658845</v>
+        <v>0.3714344482390222</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.3753520536981952</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2876</v>
+        <v>2872</v>
       </c>
       <c r="B52" t="n">
-        <v>0.3714344482390222</v>
+        <v>0.3816908723548493</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.3822033877803676</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2872</v>
+        <v>2866</v>
       </c>
       <c r="B53" t="n">
-        <v>0.3816908723548493</v>
+        <v>0.348565769238066</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.2695885480183995</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2866</v>
+        <v>2861</v>
       </c>
       <c r="B54" t="n">
-        <v>0.3411876811309565</v>
+        <v>0.3412229408875688</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.2364963427400908</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2861</v>
+        <v>2857</v>
       </c>
       <c r="B55" t="n">
-        <v>0.341215284686386</v>
+        <v>0.3824294957911895</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.2678828051140654</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2857</v>
+        <v>2850</v>
       </c>
       <c r="B56" t="n">
-        <v>0.329704553626448</v>
+        <v>0.3579566481111134</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.3558764325899996</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2850</v>
+        <v>2843</v>
       </c>
       <c r="B57" t="n">
-        <v>0.3579566481111134</v>
+        <v>0.3135601166183295</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.1829303134549639</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2843</v>
+        <v>2840</v>
       </c>
       <c r="B58" t="n">
-        <v>0.3135426413245631</v>
+        <v>0.3621813144046631</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.3094982158190912</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="B59" t="n">
-        <v>0.3621855892084546</v>
+        <v>2.604304879396142</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.08878850733104968</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="B60" t="n">
-        <v>0.4345770333206229</v>
+        <v>0.3791077949882992</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.2795475628018562</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="B61" t="n">
-        <v>0.3791077949882992</v>
+        <v>0.3497206129677597</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.1265192524180493</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="B62" t="n">
-        <v>0.3497206129677597</v>
+        <v>0.4834529714480031</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.3225488769773652</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2835</v>
+        <v>2832</v>
       </c>
       <c r="B63" t="n">
-        <v>0.3827613814466386</v>
+        <v>0.3332437817966996</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.3207110353591079</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="B64" t="n">
-        <v>0.3332437817966996</v>
+        <v>0.35594901205693</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.3267552515939188</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="B65" t="n">
-        <v>0.3559514958105615</v>
+        <v>0.3579022467365578</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.2415511146651811</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2828</v>
+        <v>2594</v>
       </c>
       <c r="B66" t="n">
-        <v>0.357900286137818</v>
+        <v>0.3870171691183409</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.2421771107376635</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2594</v>
+        <v>2554</v>
       </c>
       <c r="B67" t="n">
-        <v>0.3023962859966994</v>
+        <v>0.4007194333090533</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.3033797962161246</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2554</v>
+        <v>2527</v>
       </c>
       <c r="B68" t="n">
-        <v>0.4007209628371954</v>
+        <v>0.3749280884543377</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.2527244504894599</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2535</v>
+        <v>2517</v>
       </c>
       <c r="B69" t="n">
-        <v>0.3190059885038629</v>
+        <v>0.3698113610556444</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.2735154161934025</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2527</v>
+        <v>2516</v>
       </c>
       <c r="B70" t="n">
-        <v>0.3749137226711461</v>
+        <v>0.3510069218524295</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.2874998238539221</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2517</v>
+        <v>2378</v>
       </c>
       <c r="B71" t="n">
-        <v>0.369834391643667</v>
+        <v>0.4021462501649309</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.3015352332040474</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2516</v>
+        <v>2364</v>
       </c>
       <c r="B72" t="n">
-        <v>0.3510069218524295</v>
+        <v>0.360039719292635</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.2994914749965086</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2378</v>
+        <v>2168</v>
       </c>
       <c r="B73" t="n">
-        <v>0.3341781884027276</v>
+        <v>0.3576921311909673</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.2950274441264135</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2364</v>
+        <v>2167</v>
       </c>
       <c r="B74" t="n">
-        <v>0.3600395747971217</v>
+        <v>0.3582742137454484</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.2822159719845896</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2168</v>
+        <v>2161</v>
       </c>
       <c r="B75" t="n">
-        <v>0.3576993083941014</v>
+        <v>0.3682798786874736</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.2833219127598758</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2167</v>
+        <v>2107</v>
       </c>
       <c r="B76" t="n">
-        <v>0.3582698853645091</v>
+        <v>0.3454269318322105</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.1767351408063946</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2161</v>
+        <v>2104</v>
       </c>
       <c r="B77" t="n">
-        <v>0.3682798786874736</v>
+        <v>0.3323239723586519</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.3007119184708865</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2107</v>
+        <v>2103</v>
       </c>
       <c r="B78" t="n">
-        <v>0.345428149364334</v>
+        <v>0.3408509660557938</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.3350687471037519</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2104</v>
+        <v>2094</v>
       </c>
       <c r="B79" t="n">
-        <v>0.3324033666247075</v>
+        <v>0.3350319360420932</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.2990874840283987</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2103</v>
+        <v>2080</v>
       </c>
       <c r="B80" t="n">
-        <v>0.3408509660557938</v>
+        <v>0.2984522925637598</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.2253424006096986</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2094</v>
+        <v>2079</v>
       </c>
       <c r="B81" t="n">
-        <v>0.3350319360420932</v>
+        <v>0.4920055140540828</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.332831843028485</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>2080</v>
+        <v>2076</v>
       </c>
       <c r="B82" t="n">
-        <v>0.2984417582585155</v>
+        <v>0.4048803021393707</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.2257864059858031</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>2079</v>
+        <v>2049</v>
       </c>
       <c r="B83" t="n">
-        <v>0.3566750705912832</v>
+        <v>0.3613718015950349</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.2986295917733249</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2076</v>
+        <v>1912</v>
       </c>
       <c r="B84" t="n">
-        <v>0.4049225652738282</v>
+        <v>0.5213840596956788</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.1869888518525323</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2049</v>
+        <v>1723</v>
       </c>
       <c r="B85" t="n">
-        <v>0.3613686374968849</v>
+        <v>0.3716312694452902</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.2806189290612324</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1912</v>
+        <v>1720</v>
       </c>
       <c r="B86" t="n">
-        <v>0.5213840596956788</v>
+        <v>0.3744743974591479</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.189875698102339</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1723</v>
+        <v>1710</v>
       </c>
       <c r="B87" t="n">
-        <v>0.3543480377048764</v>
+        <v>0.3940655355512691</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.3432023137636835</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1720</v>
+        <v>1702</v>
       </c>
       <c r="B88" t="n">
-        <v>0.3744687990355599</v>
+        <v>0.3729988994955625</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.376989498882803</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1710</v>
+        <v>1619</v>
       </c>
       <c r="B89" t="n">
-        <v>0.3940655355512691</v>
+        <v>0.4822602500308986</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.3129963387890729</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1702</v>
+        <v>1606</v>
       </c>
       <c r="B90" t="n">
-        <v>0.3729988994955625</v>
+        <v>0.4111931147911536</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.2576834094500449</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1619</v>
+        <v>1573</v>
       </c>
       <c r="B91" t="n">
-        <v>0.3474482306160764</v>
+        <v>0.3850465353245314</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.318426680414835</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1606</v>
+        <v>1571</v>
       </c>
       <c r="B92" t="n">
-        <v>0.4117941486263398</v>
+        <v>0.3647835277017356</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.3263599274711367</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="B93" t="n">
-        <v>0.3850465353245314</v>
+        <v>0.3309031813868305</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.2175192469636241</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1571</v>
+        <v>1552</v>
       </c>
       <c r="B94" t="n">
-        <v>0.3647835277017356</v>
+        <v>0.3189135236987325</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.1819597408102214</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1570</v>
+        <v>1384</v>
       </c>
       <c r="B95" t="n">
-        <v>0.330896857079053</v>
+        <v>0.3709580368288992</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.3539739019315459</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>1552</v>
+        <v>1382</v>
       </c>
       <c r="B96" t="n">
-        <v>0.318912076637355</v>
+        <v>0.3091456705991906</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.06304002232048303</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="B97" t="n">
-        <v>0.3709580368288984</v>
+        <v>0.3561356106057925</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.3316217407851156</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="B98" t="n">
-        <v>0.3091456705991903</v>
+        <v>0.2602492216789122</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0.2192747352870803</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="B99" t="n">
-        <v>0.3561356106057925</v>
+        <v>0.5667705677812378</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0.1794564314696095</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="B100" t="n">
-        <v>0.2602513977872986</v>
+        <v>0.3139419296879841</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.1583872230727588</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1378</v>
+        <v>1357</v>
       </c>
       <c r="B101" t="n">
-        <v>0.3629128321583328</v>
+        <v>0.3147888834803775</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.2211515454740631</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>1374</v>
+        <v>1356</v>
       </c>
       <c r="B102" t="n">
-        <v>0.3139404239921251</v>
+        <v>0.404001646717537</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.3195114566958964</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="B103" t="n">
-        <v>0.3147928513724274</v>
+        <v>0.3487187858547596</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.3040080299850326</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>1356</v>
+        <v>1295</v>
       </c>
       <c r="B104" t="n">
-        <v>0.3339558841355669</v>
+        <v>2.05177247605194</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0.2749952266905087</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>1355</v>
+        <v>1241</v>
       </c>
       <c r="B105" t="n">
-        <v>0.3259858533473405</v>
+        <v>0.390066111243477</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0.2325610711514961</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1295</v>
+        <v>1104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.4289735484441664</v>
+        <v>0.3260176678836244</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0.1521048992032321</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1241</v>
+        <v>1081</v>
       </c>
       <c r="B107" t="n">
-        <v>0.3539409570125668</v>
+        <v>0.5507934642717458</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.342973349438488</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>1104</v>
+        <v>1073</v>
       </c>
       <c r="B108" t="n">
-        <v>0.3260159719447677</v>
+        <v>0.3825847251278167</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0.1028952642360957</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1091</v>
+        <v>1048</v>
       </c>
       <c r="B109" t="n">
-        <v>0.3581549396693045</v>
+        <v>0.3474893300106217</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0.3008380441315619</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>1081</v>
+        <v>1043</v>
       </c>
       <c r="B110" t="n">
-        <v>0.3524276991339261</v>
+        <v>0.3453720536206965</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0.3010690731983817</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>1048</v>
+        <v>1012</v>
       </c>
       <c r="B111" t="n">
-        <v>0.3474739711443442</v>
+        <v>0.3046535248917526</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0.2827103819132206</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>1043</v>
+        <v>1010</v>
       </c>
       <c r="B112" t="n">
-        <v>0.3453711311096243</v>
+        <v>0.5023904058892911</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.2494889898667585</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="B113" t="n">
-        <v>0.3046535248917545</v>
+        <v>0.2836355858900913</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.2248366001098001</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>1010</v>
+        <v>1001</v>
       </c>
       <c r="B114" t="n">
-        <v>0.3570301254695712</v>
+        <v>0.3373614043107674</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.2351861726741784</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>1008</v>
+        <v>997</v>
       </c>
       <c r="B115" t="n">
-        <v>0.283634775922768</v>
+        <v>0.3154158372992738</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.1414537313146478</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>1001</v>
+        <v>995</v>
       </c>
       <c r="B116" t="n">
-        <v>0.3373626808785843</v>
+        <v>0.3341057713080128</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0.1099034620669631</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="B117" t="n">
-        <v>0.3154158372992738</v>
+        <v>0.3193461637203914</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.3002334817384795</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="B118" t="n">
-        <v>0.3341057713080128</v>
+        <v>0.377597647224074</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0.3028253148388222</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="B119" t="n">
-        <v>0.3068714219036599</v>
+        <v>0.3200383648458848</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0.3007083663699309</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="B120" t="n">
-        <v>0.3775981724419372</v>
+        <v>0.4369362396923436</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0.219423550284241</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>990</v>
+        <v>983</v>
       </c>
       <c r="B121" t="n">
-        <v>0.3200383648458848</v>
+        <v>0.3643001584047057</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0.3554259716397997</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>988</v>
+        <v>897</v>
       </c>
       <c r="B122" t="n">
-        <v>0.3743860166334052</v>
+        <v>0.3753025580695051</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0.2080688625334745</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>983</v>
+        <v>892</v>
       </c>
       <c r="B123" t="n">
-        <v>0.3643001584047057</v>
+        <v>0.3423287839730054</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0.176354625030066</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="B124" t="n">
-        <v>0.3752821958994034</v>
+        <v>0.368209472500456</v>
+      </c>
+      <c r="C124" t="n">
+        <v>0.2468045397430277</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="B125" t="n">
-        <v>0.342328775128332</v>
+        <v>0.3217583741703381</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0.3209856327912293</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>889</v>
+        <v>876</v>
       </c>
       <c r="B126" t="n">
-        <v>0.368209472500456</v>
+        <v>0.3490808065648447</v>
+      </c>
+      <c r="C126" t="n">
+        <v>0.1408378652040445</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>887</v>
+        <v>874</v>
       </c>
       <c r="B127" t="n">
-        <v>0.3217583741703381</v>
+        <v>0.3610796311341488</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0.238954363544711</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>876</v>
+        <v>864</v>
       </c>
       <c r="B128" t="n">
-        <v>0.3490821787340423</v>
+        <v>0.3032921994982787</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0.1488743077229255</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>874</v>
+        <v>863</v>
       </c>
       <c r="B129" t="n">
-        <v>0.3426734039541678</v>
+        <v>0.3256974475820567</v>
+      </c>
+      <c r="C129" t="n">
+        <v>0.1879425499591285</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B130" t="n">
-        <v>0.3032922001446938</v>
+        <v>0.5887604521763219</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0.2349389855258899</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B131" t="n">
-        <v>0.3256886696454522</v>
+        <v>0.3167810529762386</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0.1921135570225264</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>862</v>
+        <v>733</v>
       </c>
       <c r="B132" t="n">
-        <v>0.588820722831622</v>
+        <v>0.343957426640445</v>
+      </c>
+      <c r="C132" t="n">
+        <v>0.2946109943963943</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>861</v>
+        <v>728</v>
       </c>
       <c r="B133" t="n">
-        <v>0.3167747910815306</v>
+        <v>0.3452912417166399</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0.2813944014617442</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="B134" t="n">
-        <v>0.3439551368408519</v>
+        <v>0.3493932630422841</v>
+      </c>
+      <c r="C134" t="n">
+        <v>0.2340505526158381</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>728</v>
+        <v>710</v>
       </c>
       <c r="B135" t="n">
-        <v>0.3453046485199199</v>
+        <v>0.3920208048396226</v>
+      </c>
+      <c r="C135" t="n">
+        <v>0.3084731658007794</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>727</v>
+        <v>709</v>
       </c>
       <c r="B136" t="n">
-        <v>0.3412756417373134</v>
+        <v>0.3770303255745312</v>
+      </c>
+      <c r="C136" t="n">
+        <v>0.417394023590101</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B137" t="n">
-        <v>0.3920177962687497</v>
+        <v>0.3532671931796519</v>
+      </c>
+      <c r="C137" t="n">
+        <v>0.2801051729978689</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="B138" t="n">
-        <v>0.3770283805511454</v>
+        <v>0.3692771382504424</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0.2522378242698015</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>708</v>
+        <v>699</v>
       </c>
       <c r="B139" t="n">
-        <v>0.3532885604993627</v>
+        <v>0.4209821611508353</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0.2431552076022918</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>703</v>
+        <v>645</v>
       </c>
       <c r="B140" t="n">
-        <v>0.3692435881529905</v>
+        <v>0.3350241609741931</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.2930353422789901</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>699</v>
+        <v>642</v>
       </c>
       <c r="B141" t="n">
-        <v>0.4207523166318731</v>
+        <v>0.2647797501931667</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.1664603001366493</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B142" t="n">
-        <v>0.3350241609741931</v>
+        <v>0.3958268962092519</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0.3236362580725322</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>642</v>
+        <v>47</v>
       </c>
       <c r="B143" t="n">
-        <v>0.2647823733792366</v>
+        <v>0.3519491089564129</v>
+      </c>
+      <c r="C143" t="n">
+        <v>0.3319633994983702</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>641</v>
+        <v>26</v>
       </c>
       <c r="B144" t="n">
-        <v>0.3958268962092519</v>
+        <v>0.3505273733544978</v>
+      </c>
+      <c r="C144" t="n">
+        <v>0.2801632709223243</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B145" t="n">
-        <v>0.3519491089564129</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="n">
-        <v>26</v>
-      </c>
-      <c r="B146" t="n">
-        <v>0.3505273733544978</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="n">
-        <v>7</v>
-      </c>
-      <c r="B147" t="n">
-        <v>0.2758370902002062</v>
+        <v>0.2758229919721963</v>
+      </c>
+      <c r="C145" t="n">
+        <v>0.1188680437542776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>